<commit_message>
new file:   Brighway/Monte_Carlo.py 	modified:   Brighway/Results/Ananas - CONSQ.xlsx 	modified:   Brighway/Results/Ananas sub - CONSQ.xlsx 	modified:   Brighway/Rune BE.ipynb 	modified:   Brighway/Rune_contribution.ipynb 	new file:   Brighway/__pycache__/Monte_Carlo.cpython-311.pyc
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ.xlsx
+++ b/Brighway/Results/Ananas - CONSQ.xlsx
@@ -64,148 +64,148 @@
     <t>('EF v3.1 EN15804', 'water use', 'user deprivation potential (deprivation-weighted water consumption)')</t>
   </si>
   <si>
-    <t>[["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.033706295500991905], ["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase CDU", 0.0011995761189752317], ["EoL CDU", 0.009568273319826437], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0690910181269958], ["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase MDU", 0.0004519679633273833], ["EoL MDU", 0.023743427245292378], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase basecase", 227.34409189224243], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.12905040685291852], ["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase CDU", 43.44535637749612], ["EoL CDU", -0.010913517128917348], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.3591249305157672], ["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase MDU", 43.404329830374245], ["EoL MDU", -0.028320516611116342], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4899964112890802], ["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase CDU", 0.7412027382979668], ["EoL CDU", -0.21693100903846793], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.562379936011466], ["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase MDU", 0.2792652227250268], ["EoL MDU", -0.5284116708803903], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.1050843577039284], ["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase CDU", 0.6692525251663012], ["EoL CDU", -0.09497370330413925], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.548337101555568], ["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase MDU", 0.2521563208589757], ["EoL MDU", -0.22894948284262986], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.00011021647529885492], ["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase CDU", 2.849641883711377e-05], ["EoL CDU", -2.051417753377876e-05], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0003663742164220076], ["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase MDU", 1.0736682883398692e-05], ["EoL MDU", -4.919735864856039e-05], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.0001277696567481476], ["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase CDU", 0.0002792513031362428], ["EoL CDU", -7.792099234694213e-05], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0003618564128267861], ["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase MDU", 0.00010521436759080808], ["EoL MDU", -0.0001918865112239045], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.001305192214177572], ["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase CDU", 0.00435189277730263], ["EoL CDU", -0.0011410749274370425], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.00376108667227394], ["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase MDU", 0.0016396759522497191], ["EoL MDU", -0.0028112447635443957], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 3.243928866899465e-10], ["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase CDU", 3.112433080829649e-10], ["EoL CDU", -1.382464959096833e-10], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.0716849153781413e-09], ["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase MDU", 1.1726809314424572e-10], ["EoL MDU", -3.4273432030762576e-10], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase basecase", 1.3361670158765134e-08], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 4.681941563932091e-09], ["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase CDU", 1.1108940558494202e-08], ["EoL CDU", -7.86491525690251e-09], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.1984131040941075e-08], ["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase MDU", 5.774491740088175e-09], ["EoL MDU", -1.9440126151375635e-08], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.02299027511022214], ["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase CDU", 0.0003478036811559822], ["EoL CDU", 0.0005368187911133735], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.05186765582859973], ["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase MDU", 0.00013104305672618255], ["EoL MDU", 0.0013724670382122136], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4517019264400177], ["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase CDU", 30.062931902825287], ["EoL CDU", -0.5926562572475528], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 3.6900959245079963], ["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase MDU", 11.326902802466671], ["EoL MDU", -1.4269104476387922], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.336491107311484e-05], ["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase CDU", 9.734411970101328e-06], ["EoL CDU", -6.048185424361905e-06], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 7.762141349179897e-05], ["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase MDU", 3.6676641713034824e-06], ["EoL MDU", -1.4385742203969544e-05], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 6.448093853719628e-09], ["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase CDU", 1.9450074606027338e-09], ["EoL CDU", 7.567022242406086e-12], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.8962760185799554e-08], ["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase MDU", 7.328264098676998e-10], ["EoL MDU", 1.5588458631096705e-11], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.9230755321320073e-08], ["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase CDU", 1.3992546509704515e-08], ["EoL CDU", 5.258378664716782e-09], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 6.342169280575578e-08], ["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase MDU", 5.272014545569526e-09], ["EoL MDU", 1.3037019606857843e-08], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.0026820678763302087], ["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase CDU", 0.0008604984653688513], ["EoL CDU", 0.00034483736920948576], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.005810953630409368], ["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase MDU", 0.00032421263868720836], ["EoL MDU", 0.0008591276393808767], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.04630923474954789], ["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase CDU", 0.026577952308437253], ["EoL CDU", 0.005541157071511327], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.12369240377069371], ["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase MDU", 0.01001385638163526], ["EoL MDU", 0.01385106430137736], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
+    <t>[["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.033699763481384294], ["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase CDU", 0.0011995761189071566], ["EoL CDU", 0.0012242722397637902], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.06909101812686011], ["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase MDU", 0.00045196796330177], ["EoL MDU", 0.007055424060427032], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase basecase", 227.34409189224243], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.12819826622266475], ["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase CDU", 43.445356377489226], ["EoL CDU", -0.00030258188038357025], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.3591249304907266], ["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase MDU", 43.404329830371644], ["EoL MDU", -0.0070986448114089525], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 1.4755335896694415], ["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase CDU", 0.7412027382264046], ["EoL CDU", -0.004626877616344883], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 5.562379935751366], ["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase MDU", 0.2792652226980472], ["EoL MDU", -0.10380338196557717], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 2.094289083153275], ["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase CDU", 0.6692525250789959], ["EoL CDU", 0.0023623570522492655], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 5.548337101274091], ["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase MDU", 0.2521563208261186], ["EoL MDU", -0.03427735018172776], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.00010946578693302614], ["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase CDU", 2.849641883337073e-05], ["EoL CDU", -6.603880166606268e-07], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.0003663742164005576], ["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase MDU", 1.073668288198834e-05], ["EoL MDU", -9.489777176417246e-06], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.00012323944886451918], ["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase CDU", 0.00027925130312526306], ["EoL CDU", -6.2441110170754856e-06], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.000361856412791819], ["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase MDU", 0.00010521436758666906], ["EoL MDU", -4.8532739762006666e-05], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.001291805268237013], ["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase CDU", 0.004351892777136212], ["EoL CDU", -9.307467647554836e-05], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.0037610866718165645], ["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase MDU", 0.0016396759521870126], ["EoL MDU", -0.0007152441329165199], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 3.23120762737068e-10], ["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase CDU", 3.112433080587344e-10], ["EoL CDU", -7.707922940565687e-12], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 1.0716849152239044e-09], ["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase MDU", 1.1726809313497473e-10], ["EoL MDU", -8.165715833980981e-11], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase basecase", 1.3361670158765134e-08], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 4.527936227184927e-09], ["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase CDU", 1.1108940558000346e-08], ["EoL CDU", -2.91480127867933e-10], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 1.1984131035265172e-08], ["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase MDU", 5.7744917398854014e-09], ["EoL MDU", -4.293254963228643e-09], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.022953633802310615], ["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase CDU", 0.00034780368107774893], ["EoL CDU", 0.00011107874461068391], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.05186765582765432], ["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase MDU", 0.00013104305669854347], ["EoL MDU", 0.0005209868928899672], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 1.4453593855555278], ["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase CDU", 30.062931903317136], ["EoL CDU", -0.02832465624823723], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 3.6900959224740673], ["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase MDU", 11.326902802631512], ["EoL MDU", -0.29824717604918993], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 2.3204757355396628e-05], ["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase CDU", 9.73441196893503e-06], ["EoL CDU", 7.408005945760737e-07], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 7.762141348560289e-05], ["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase MDU", 3.6676641708639582e-06], ["EoL MDU", -8.07769332375321e-07], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 6.412188285949878e-09], ["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase CDU", 1.9450074604811147e-09], ["EoL CDU", 1.3108767544701095e-11], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 1.8962760185311458e-08], ["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase MDU", 7.328264098056545e-10], ["EoL MDU", 2.667194990667454e-11], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 2.9190976038666193e-08], ["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase CDU", 1.3992546508923827e-08], ["EoL CDU", 7.644866224450964e-10], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 6.342169280380604e-08], ["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase MDU", 5.272014545275251e-09], ["EoL MDU", 4.049234970385121e-09], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.002678400846522548], ["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase CDU", 0.0008604984653242085], ["EoL CDU", 5.4636027418626265e-05], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.005810953630291378], ["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase MDU", 0.000324212638670387], ["EoL MDU", 0.0002787249201572001], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
+  </si>
+  <si>
+    <t>[["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
+  </si>
+  <si>
+    <t>[["CDU updated", 0.04610221142028905], ["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase CDU", 0.026577952306826722], ["EoL CDU", 0.000897610415032529], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
+  </si>
+  <si>
+    <t>[["MDU updated", 0.1236924037638626], ["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase MDU", 0.01001385638102837], ["EoL MDU", 0.004563970418034172], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ.xlsx 	modified:   Brighway/Results/Ananas - test.xlsx 	new file:   Brighway/Results/Ananas contribution - CONSQ.xlsx 	modified:   Brighway/Rune BE.ipynb 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_CDU.jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_MDU.jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_No DU.jpg 	modified:   Brighway/Stine BE.ipynb 	modified:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/climate change -monte_carlo_simulations_Rune.xlsx 	new file:   Brighway/df_idx_ofir 	modified:   Brighway/impact_categories 	modified:   Brighway/life_cycle_assessment.py
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ.xlsx
+++ b/Brighway/Results/Ananas - CONSQ.xlsx
@@ -64,148 +64,148 @@
     <t>('EF v3.1 EN15804', 'water use', 'user deprivation potential (deprivation-weighted water consumption)')</t>
   </si>
   <si>
-    <t>[["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.033699763481384294], ["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase CDU", 0.0011995761189071566], ["EoL CDU", 0.0012242722397637902], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.06909101812686011], ["Steel cylinder", 2.4821260976820004e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase MDU", 0.00045196796330177], ["EoL MDU", 0.007055424060427032], ["EoL 50L cylinder - FU", 0.0015934554481004321]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase basecase", 227.34409189224243], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.12819826622266475], ["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase CDU", 43.445356377489226], ["EoL CDU", -0.00030258188038357025], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.3591249304907266], ["Steel cylinder", 0.005456229514756893], ["nitrous oxide production", 2.7735767368862367], ["Use phase MDU", 43.404329830371644], ["EoL MDU", -0.0070986448114089525], ["EoL 50L cylinder - FU", 1.3797549866934615]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4755335896694415], ["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase CDU", 0.7412027382264046], ["EoL CDU", -0.004626877616344883], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.562379935751366], ["Steel cylinder", 0.02689681145503979], ["nitrous oxide production", 15.635308294302359], ["Use phase MDU", 0.2792652226980472], ["EoL MDU", -0.10380338196557717], ["EoL 50L cylinder - FU", 2.5968806464953906]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.094289083153275], ["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase CDU", 0.6692525250789959], ["EoL CDU", 0.0023623570522492655], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.548337101274091], ["Steel cylinder", 0.06471586600422786], ["nitrous oxide production", 46.31028189903245], ["Use phase MDU", 0.2521563208261186], ["EoL MDU", -0.03427735018172776], ["EoL 50L cylinder - FU", 6.953517004338244]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.00010946578693302614], ["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase CDU", 2.849641883337073e-05], ["EoL CDU", -6.603880166606268e-07], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0003663742164005576], ["Steel cylinder", 4.164145755153704e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase MDU", 1.073668288198834e-05], ["EoL MDU", -9.489777176417246e-06], ["EoL 50L cylinder - FU", 0.0001231153606355252]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.00012323944886451918], ["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase CDU", 0.00027925130312526306], ["EoL CDU", -6.2441110170754856e-06], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.000361856412791819], ["Steel cylinder", 5.439366377934605e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase MDU", 0.00010521436758666906], ["EoL MDU", -4.8532739762006666e-05], ["EoL 50L cylinder - FU", 0.0006537394847833525]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.001291805268237013], ["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase CDU", 0.004351892777136212], ["EoL CDU", -9.307467647554836e-05], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0037610866718165645], ["Steel cylinder", 5.1440088432858044e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase MDU", 0.0016396759521870126], ["EoL MDU", -0.0007152441329165199], ["EoL 50L cylinder - FU", 0.004205256078726926]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 3.23120762737068e-10], ["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase CDU", 3.112433080587344e-10], ["EoL CDU", -7.707922940565687e-12], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.0716849152239044e-09], ["Steel cylinder", 8.120702205798173e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase MDU", 1.1726809313497473e-10], ["EoL MDU", -8.165715833980981e-11], ["EoL 50L cylinder - FU", 2.4542745026166035e-10]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase basecase", 1.3361670158765134e-08], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 4.527936227184927e-09], ["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase CDU", 1.1108940558000346e-08], ["EoL CDU", -2.91480127867933e-10], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.1984131035265172e-08], ["Steel cylinder", 6.725000501277105e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase MDU", 5.7744917398854014e-09], ["EoL MDU", -4.293254963228643e-09], ["EoL 50L cylinder - FU", 5.05522698476935e-09]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.022953633802310615], ["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase CDU", 0.00034780368107774893], ["EoL CDU", 0.00011107874461068391], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.05186765582765432], ["Steel cylinder", 3.451402200181894e-05], ["nitrous oxide production", 0.42490983327819815], ["Use phase MDU", 0.00013104305669854347], ["EoL MDU", 0.0005209868928899672], ["EoL 50L cylinder - FU", 0.052218194515324355]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4453593855555278], ["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase CDU", 30.062931903317136], ["EoL CDU", -0.02832465624823723], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 3.6900959224740673], ["Steel cylinder", 0.05341058184255911], ["nitrous oxide production", 28.792690550160245], ["Use phase MDU", 11.326902802631512], ["EoL MDU", -0.29824717604918993], ["EoL 50L cylinder - FU", 4.553405133415671]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.3204757355396628e-05], ["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase CDU", 9.73441196893503e-06], ["EoL CDU", 7.408005945760737e-07], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 7.762141348560289e-05], ["Steel cylinder", -6.260798244751308e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase MDU", 3.6676641708639582e-06], ["EoL MDU", -8.07769332375321e-07], ["EoL 50L cylinder - FU", 5.124795525628333e-06]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 6.412188285949878e-09], ["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase CDU", 1.9450074604811147e-09], ["EoL CDU", 1.3108767544701095e-11], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.8962760185311458e-08], ["Steel cylinder", 1.232676817653973e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase MDU", 7.328264098056545e-10], ["EoL MDU", 2.667194990667454e-11], ["EoL 50L cylinder - FU", 1.043284139163744e-07]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.9190976038666193e-08], ["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase CDU", 1.3992546508923827e-08], ["EoL CDU", 7.644866224450964e-10], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 6.342169280380604e-08], ["Steel cylinder", 5.476745429210785e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase MDU", 5.272014545275251e-09], ["EoL MDU", 4.049234970385121e-09], ["EoL 50L cylinder - FU", 1.604819459417503e-08]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.002678400846522548], ["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase CDU", 0.0008604984653242085], ["EoL CDU", 5.4636027418626265e-05], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.005810953630291378], ["Steel cylinder", 2.334134230290092e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase MDU", 0.000324212638670387], ["EoL MDU", 0.0002787249201572001], ["EoL 50L cylinder - FU", 0.0012673930560681216]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.04610221142028905], ["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase CDU", 0.026577952306826722], ["EoL CDU", 0.000897610415032529], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.1236924037638626], ["Steel cylinder", 0.0015157174317935512], ["nitrous oxide production", 4.430496838846222], ["Use phase MDU", 0.01001385638102837], ["EoL MDU", 0.004563970418034172], ["EoL 50L cylinder - FU", 0.4699444626920632]]</t>
+    <t>[["alubox raw materials - CONSQ", 0.0009945931379171746], ["alubox production - CONSQ", 9.762607499157567e-05], ["autoclave - CONSQ", 0.001401428541323231], ["disinfection - CONSQ", 0.0014088446645906597], ["Handwash - CONSQ", 0.00013896582908387405], ["alubox EoL melting - CONSQ", 0.000863221102808307], ["alubox EoL mixed sorting - CONSQ", 1.3102513605718994e-05], ["transport Alu - CONSQ", 5.1128321043765874e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955792616025], ["autoclave - CONSQ", 0.001401428541323231], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["market for electricity, high voltage", -0.00010747647019143262], ["transport Plastic - CONSQ", 0.0005506473682877801], ["PE incineration no Energy Recovery - CONSQ", 3.9754072547888845e-06], ["PP incineration no Energy Recovery - CONSQ", 2.9272704199409187e-05], ["marginal heating grid projection updated - CONSQ", -0.0003627581959658382]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955792616025], ["autoclave - CONSQ", 0.001401428541323231], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.943299789376843e-05], ["market for polypropylene, granulate", -0.00032980866027868883], ["market for electricity, high voltage", -4.9439176288059175e-05], ["transport Plastic - CONSQ", 0.0005506473682877801], ["PE incineration no Energy Recovery - CONSQ", 1.8286873392296424e-06], ["PP incineration no Energy Recovery - CONSQ", 1.3465443823057513e-05], ["marginal heating grid projection updated - CONSQ", -0.00016686877007444426]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.15424392822864008], ["alubox production - CONSQ", 0.022156774009621943], ["autoclave - CONSQ", 0.13321320167037295], ["disinfection - CONSQ", 0.08963416459471302], ["Handwash - CONSQ", 0.02337957579346481], ["alubox EoL melting - CONSQ", 0.13106909346999387], ["alubox EoL mixed sorting - CONSQ", 0.0031809502669847747], ["transport Alu - CONSQ", 0.0021324672021639807]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.22940403947612345], ["autoclave - CONSQ", 0.13321320167037295], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["market for electricity, high voltage", -0.005961318604063036], ["transport Plastic - CONSQ", 0.060764277659934196], ["PE incineration no Energy Recovery - CONSQ", 0.03039316708934747], ["PP incineration no Energy Recovery - CONSQ", 0.2223142905005214], ["marginal heating grid projection updated - CONSQ", -0.15272040511343357]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.22940403947612345], ["autoclave - CONSQ", 0.13321320167037295], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011359305107549338], ["market for polypropylene, granulate", -0.09625534407615824], ["market for electricity, high voltage", -0.002742206557869834], ["transport Plastic - CONSQ", 0.060764277659934196], ["PE incineration no Energy Recovery - CONSQ", 0.013980856861259182], ["PP incineration no Energy Recovery - CONSQ", 0.10226457362246834], ["marginal heating grid projection updated - CONSQ", -0.0702513863552857]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.5100605935727014], ["alubox production - CONSQ", 0.11210832105151619], ["autoclave - CONSQ", 1.4495155523989065], ["disinfection - CONSQ", 1.2663943622657485], ["Handwash - CONSQ", 1.4404524083329517], ["alubox EoL melting - CONSQ", 0.24075710948842505], ["alubox EoL mixed sorting - CONSQ", 0.0175132391793385], ["transport Alu - CONSQ", 0.014308575806399947]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917564937834], ["autoclave - CONSQ", 1.4495155523989065], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["market for electricity, high voltage", -0.05148097890038078], ["transport Plastic - CONSQ", 0.41868503474150837], ["PE incineration no Energy Recovery - CONSQ", 0.005492658538918375], ["PP incineration no Energy Recovery - CONSQ", 0.040469513083771405], ["marginal heating grid projection updated - CONSQ", -0.19814111293767944]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917564937834], ["autoclave - CONSQ", 1.4495155523989065], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.014617415777911277], ["market for polypropylene, granulate", -0.11847606457727207], ["market for electricity, high voltage", -0.023681250294174457], ["transport Plastic - CONSQ", 0.41868503474150837], ["PE incineration no Energy Recovery - CONSQ", 0.0025266229295744123], ["PP incineration no Energy Recovery - CONSQ", 0.018615975931685874], ["marginal heating grid projection updated - CONSQ", -0.09114491198797947]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.5044803926965291], ["alubox production - CONSQ", 0.3314053978562584], ["autoclave - CONSQ", 2.6222095073851883], ["disinfection - CONSQ", 0.9614618910155737], ["Handwash - CONSQ", 0.20052001646412607], ["alubox EoL melting - CONSQ", 1.2546444967552859], ["alubox EoL mixed sorting - CONSQ", 0.03342991772325342], ["transport Alu - CONSQ", 0.03016378175125673]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.1063850688446575], ["autoclave - CONSQ", 2.6222095073851883], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["market for electricity, high voltage", -0.06451435176929034], ["transport Plastic - CONSQ", 0.7661470104554844], ["PE incineration no Energy Recovery - CONSQ", 0.004737511073583869], ["PP incineration no Energy Recovery - CONSQ", 0.03531591964766336], ["marginal heating grid projection updated - CONSQ", -1.9042468330459614]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.1063850688446575], ["autoclave - CONSQ", 2.6222095073851883], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.3917069938836761], ["market for polypropylene, granulate", -3.455013830627775], ["market for electricity, high voltage", -0.029676601813876657], ["transport Plastic - CONSQ", 0.7661470104554844], ["PE incineration no Energy Recovery - CONSQ", 0.002179255096051083], ["PP incineration no Energy Recovery - CONSQ", 0.016245322935529587], ["marginal heating grid projection updated - CONSQ", -0.8759535432763497]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.674180468862365e-05], ["alubox production - CONSQ", 1.3995384524358032e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["disinfection - CONSQ", 3.5584880575219164e-05], ["Handwash - CONSQ", 0.00018762709538521408], ["alubox EoL melting - CONSQ", 4.4898802320666606e-05], ["alubox EoL mixed sorting - CONSQ", 2.9157591258433636e-06], ["transport Alu - CONSQ", 2.1641692036306876e-07]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.6445483987961924e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["market for electricity, high voltage", -2.3521884456291384e-06], ["transport Plastic - CONSQ", 1.3662180517295428e-05], ["PE incineration no Energy Recovery - CONSQ", 4.702523210284834e-08], ["PP incineration no Energy Recovery - CONSQ", 3.7275612579358277e-07], ["marginal heating grid projection updated - CONSQ", -2.3048939664613542e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.6445483987961924e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3834463252213407e-06], ["market for polypropylene, granulate", -1.0607017560192631e-05], ["market for electricity, high voltage", -1.0820066849895143e-06], ["transport Plastic - CONSQ", 1.3662180517295428e-05], ["PE incineration no Energy Recovery - CONSQ", 2.1631606855422463e-08], ["PP incineration no Energy Recovery - CONSQ", 1.7146781393715555e-07], ["marginal heating grid projection updated - CONSQ", -1.0602512243667338e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.000163881654485523], ["alubox production - CONSQ", 2.0912907037267336e-05], ["autoclave - CONSQ", 0.0005318438000221372], ["disinfection - CONSQ", 0.00044366254416675034], ["Handwash - CONSQ", 0.0003436229861670134], ["alubox EoL melting - CONSQ", 0.0001420371138268665], ["alubox EoL mixed sorting - CONSQ", 3.073223870126413e-06], ["transport Alu - CONSQ", 1.3826016473134355e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256543071508], ["autoclave - CONSQ", 0.0005318438000221372], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["market for electricity, high voltage", -2.959148606151654e-05], ["transport Plastic - CONSQ", 0.0002401220652228008], ["PE incineration no Energy Recovery - CONSQ", 2.0429818231506584e-06], ["PP incineration no Energy Recovery - CONSQ", 1.499103348869123e-05], ["marginal heating grid projection updated - CONSQ", -0.00011074079953044283]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256543071508], ["autoclave - CONSQ", 0.0005318438000221372], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.495174878614386e-06], ["market for polypropylene, granulate", -6.876059319507486e-05], ["market for electricity, high voltage", -1.3612083588297858e-05], ["transport Plastic - CONSQ", 0.0002401220652228008], ["PE incineration no Energy Recovery - CONSQ", 9.397716389335705e-07], ["PP incineration no Energy Recovery - CONSQ", 6.89587539076395e-06], ["marginal heating grid projection updated - CONSQ", -5.094076778732855e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0017368917598334101], ["alubox production - CONSQ", 0.0001856808626641268], ["autoclave - CONSQ", 0.006227844001905327], ["disinfection - CONSQ", 0.005904113186690734], ["Handwash - CONSQ", 0.00047487836259920807], ["alubox EoL melting - CONSQ", 0.0014965946551747942], ["alubox EoL mixed sorting - CONSQ", 3.0447073785008677e-05], ["transport Alu - CONSQ", 1.4256163138019514e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486061642647], ["autoclave - CONSQ", 0.006227844001905327], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["market for electricity, high voltage", -0.0004665919463496633], ["transport Plastic - CONSQ", 0.00260272582979734], ["PE incineration no Energy Recovery - CONSQ", 2.0857587867818552e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0001530665074619661], ["marginal heating grid projection updated - CONSQ", -0.0012188533129356054]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486061642647], ["autoclave - CONSQ", 0.006227844001905327], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.009658202656336e-05], ["market for polypropylene, granulate", -0.0007317515213936433], ["market for electricity, high voltage", -0.00021463229532084788], ["transport Plastic - CONSQ", 0.00260272582979734], ["PE incineration no Energy Recovery - CONSQ", 9.594490423206304e-06], ["PP incineration no Energy Recovery - CONSQ", 7.041059322068724e-05], ["marginal heating grid projection updated - CONSQ", -0.0005606725240835317]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.602823240611735e-10], ["alubox production - CONSQ", 5.309861270471534e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["disinfection - CONSQ", 3.6409678363480453e-10], ["Handwash - CONSQ", 4.322849503680417e-11], ["alubox EoL melting - CONSQ", 2.638370965941138e-10], ["alubox EoL mixed sorting - CONSQ", -1.345407722378956e-11], ["transport Alu - CONSQ", 1.1754579073721845e-12]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115427464358e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["market for electricity, high voltage", -2.5871319984405878e-11], ["transport Plastic - CONSQ", 5.3489867490061055e-11], ["PE incineration no Energy Recovery - CONSQ", 7.115851227019668e-13], ["PP incineration no Energy Recovery - CONSQ", 5.494110762407928e-12], ["marginal heating grid projection updated - CONSQ", -9.417353664137237e-11]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115427464358e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.813968395074686e-12], ["market for polypropylene, granulate", -2.864684992177723e-11], ["market for electricity, high voltage", -1.190080719282235e-11], ["transport Plastic - CONSQ", 5.3489867490061055e-11], ["PE incineration no Energy Recovery - CONSQ", 3.273291569813087e-13], ["PP incineration no Energy Recovery - CONSQ", 2.5272909245026176e-12], ["marginal heating grid projection updated - CONSQ", -4.3319826845504436e-11]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.7867630139694007e-09], ["alubox production - CONSQ", 2.906200254463529e-10], ["autoclave - CONSQ", 8.116257548155443e-09], ["disinfection - CONSQ", 7.46019371490762e-09], ["Handwash - CONSQ", 1.3069723084130544e-09], ["alubox EoL melting - CONSQ", 2.029093983188106e-09], ["alubox EoL mixed sorting - CONSQ", 1.4327770049663526e-11], ["transport Alu - CONSQ", 2.203031249443254e-11]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.940653426127992e-09], ["autoclave - CONSQ", 8.116257548155443e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["market for electricity, high voltage", -5.330945378301465e-10], ["transport Plastic - CONSQ", 3.934257356952707e-10], ["PE incineration no Energy Recovery - CONSQ", 2.3717512826915464e-11], ["PP incineration no Energy Recovery - CONSQ", 1.7359564756098446e-10], ["marginal heating grid projection updated - CONSQ", -1.565397456200232e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.940653426127992e-09], ["autoclave - CONSQ", 8.116257548155443e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.698861310212956e-11], ["market for polypropylene, granulate", -6.276531983150668e-10], ["market for electricity, high voltage", -2.452234874012752e-10], ["transport Plastic - CONSQ", 3.934257356952707e-10], ["PE incineration no Energy Recovery - CONSQ", 1.0910055918006766e-11], ["PP incineration no Energy Recovery - CONSQ", 7.985399691032916e-11], ["marginal heating grid projection updated - CONSQ", -7.200828280372583e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0006450722467587322], ["alubox production - CONSQ", 0.0019047788572722536], ["autoclave - CONSQ", -0.00521719640790275], ["disinfection - CONSQ", 0.000470792032781366], ["Handwash - CONSQ", 0.001755590569259854], ["alubox EoL melting - CONSQ", 0.0012467999068701253], ["alubox EoL mixed sorting - CONSQ", -0.00014755172647712224], ["transport Alu - CONSQ", 1.0961680168464363e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999209003], ["autoclave - CONSQ", -0.00521719640790275], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["market for electricity, high voltage", -1.6945325686799705e-05], ["transport Plastic - CONSQ", 0.0002710560820291955], ["PE incineration no Energy Recovery - CONSQ", 3.125204459109416e-07], ["PP incineration no Energy Recovery - CONSQ", 1.7490279055748393e-06], ["marginal heating grid projection updated - CONSQ", -0.009521264122831089]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999209003], ["autoclave - CONSQ", -0.00521719640790275], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00022157206170105202], ["market for polypropylene, granulate", -0.0015468389680720798], ["market for electricity, high voltage", -7.794849815918213e-06], ["transport Plastic - CONSQ", 0.0002710560820291955], ["PE incineration no Energy Recovery - CONSQ", 1.4375940582638368e-07], ["PP incineration no Energy Recovery - CONSQ", 8.045527635579575e-07], ["marginal heating grid projection updated - CONSQ", -0.004379781496367154]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.3349731984572754], ["alubox production - CONSQ", 0.3812108164908996], ["autoclave - CONSQ", 42.497287921125405], ["disinfection - CONSQ", 41.68159582891549], ["Handwash - CONSQ", 0.9278423208700517], ["alubox EoL melting - CONSQ", 0.17506952519707022], ["alubox EoL mixed sorting - CONSQ", 0.004021728747484901], ["transport Alu - CONSQ", 0.018747663837717685]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591399766346], ["autoclave - CONSQ", 42.497287921125405], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["market for electricity, high voltage", -3.385238115609151], ["transport Plastic - CONSQ", 0.49202641391776436], ["PE incineration no Energy Recovery - CONSQ", -0.0005517467070879679], ["PP incineration no Energy Recovery - CONSQ", -0.003848634491936366], ["marginal heating grid projection updated - CONSQ", -4.188613614711568]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591399766346], ["autoclave - CONSQ", 42.497287921125405], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.01990280748454917], ["market for polypropylene, granulate", -0.16512423556264405], ["market for electricity, high voltage", -1.5572095331801954], ["transport Plastic - CONSQ", 0.49202641391776436], ["PE incineration no Energy Recovery - CONSQ", -0.000253803430773661], ["PP incineration no Energy Recovery - CONSQ", -0.0017703723252276253], ["marginal heating grid projection updated - CONSQ", -1.9267622649850056]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.5988961824265972e-07], ["alubox production - CONSQ", 2.2129992279305888e-07], ["autoclave - CONSQ", 6.577814174539491e-06], ["disinfection - CONSQ", 6.04683667379469e-06], ["Handwash - CONSQ", 1.995155195350066e-07], ["alubox EoL melting - CONSQ", -1.001845982851653e-06], ["alubox EoL mixed sorting - CONSQ", -2.38502064057568e-07], ["transport Alu - CONSQ", 4.203508200187605e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.3437873386267166e-06], ["autoclave - CONSQ", 6.577814174539491e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["market for electricity, high voltage", -3.8494146819582574e-07], ["transport Plastic - CONSQ", -8.189405999431164e-08], ["PE incineration no Energy Recovery - CONSQ", -1.6013953846098283e-09], ["PP incineration no Energy Recovery - CONSQ", -1.300532356531317e-08], ["marginal heating grid projection updated - CONSQ", -1.6647590262392704e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.3437873386267166e-06], ["autoclave - CONSQ", 6.577814174539491e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.0160051104600511e-07], ["market for polypropylene, granulate", -8.572124772542587e-07], ["market for electricity, high voltage", -1.7707307537004648e-07], ["transport Plastic - CONSQ", -8.189405999431164e-08], ["PE incineration no Energy Recovery - CONSQ", -7.366418438366595e-10], ["PP incineration no Energy Recovery - CONSQ", -5.982450728470476e-09], ["marginal heating grid projection updated - CONSQ", -7.657891482674546e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.346870114932336e-09], ["alubox production - CONSQ", 6.546061516729629e-10], ["autoclave - CONSQ", 5.322695918253996e-09], ["disinfection - CONSQ", 2.2179209318865375e-09], ["Handwash - CONSQ", 7.056252772238615e-10], ["alubox EoL melting - CONSQ", 9.80115744208019e-10], ["alubox EoL mixed sorting - CONSQ", 8.434689712810406e-11], ["transport Alu - CONSQ", 4.8640333822238504e-11]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.2672307267425193e-09], ["autoclave - CONSQ", 5.322695918253996e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["market for electricity, high voltage", -1.2104405225218283e-10], ["transport Plastic - CONSQ", 8.958388317628765e-10], ["PE incineration no Energy Recovery - CONSQ", 1.5639344084501915e-11], ["PP incineration no Energy Recovery - CONSQ", 1.1576338377537581e-10], ["marginal heating grid projection updated - CONSQ", -1.2743144554935814e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.2672307267425193e-09], ["autoclave - CONSQ", 5.322695918253996e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.1699072692562864e-10], ["market for polypropylene, granulate", -7.950858434997455e-10], ["market for electricity, high voltage", -5.568026403590827e-11], ["transport Plastic - CONSQ", 8.958388317628765e-10], ["PE incineration no Energy Recovery - CONSQ", 7.194098282618044e-12], ["PP incineration no Energy Recovery - CONSQ", 5.325115637008286e-11], ["marginal heating grid projection updated - CONSQ", -5.861846495403271e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.2379513986357882e-08], ["alubox production - CONSQ", 6.17038724902976e-10], ["autoclave - CONSQ", 1.7848307122014812e-08], ["disinfection - CONSQ", 1.821998482194627e-08], ["Handwash - CONSQ", 2.1520410437413735e-09], ["alubox EoL melting - CONSQ", 1.1187702333687963e-08], ["alubox EoL mixed sorting - CONSQ", 1.9362435943939807e-10], ["transport Alu - CONSQ", 1.5196424176911972e-10]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.0430954978932512e-08], ["autoclave - CONSQ", 1.7848307122014812e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["market for electricity, high voltage", -1.4253562039393767e-09], ["transport Plastic - CONSQ", 5.884235184610808e-09], ["PE incineration no Energy Recovery - CONSQ", 1.549660557939171e-11], ["PP incineration no Energy Recovery - CONSQ", 1.3628019230621342e-10], ["marginal heating grid projection updated - CONSQ", -9.508157486501743e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.0430954978932512e-08], ["autoclave - CONSQ", 1.7848307122014812e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.747443612396433e-10], ["market for polypropylene, granulate", -4.0611447739453945e-09], ["market for electricity, high voltage", -6.55663853812118e-10], ["transport Plastic - CONSQ", 5.884235184610808e-09], ["PE incineration no Energy Recovery - CONSQ", 7.128438588213649e-12], ["PP incineration no Energy Recovery - CONSQ", 6.268888743349566e-11], ["marginal heating grid projection updated - CONSQ", -4.373752444499595e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005788419782736742], ["alubox production - CONSQ", 7.128328313713283e-05], ["autoclave - CONSQ", 0.001401066316311216], ["disinfection - CONSQ", 0.001157865918747418], ["Handwash - CONSQ", 9.142048860869044e-05], ["alubox EoL melting - CONSQ", 0.000487494665781496], ["alubox EoL mixed sorting - CONSQ", 1.7801678607102722e-05], ["transport Alu - CONSQ", 7.90076841276903e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374024618735], ["autoclave - CONSQ", 0.001401066316311216], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["market for electricity, high voltage", -8.942695806091347e-05], ["transport Plastic - CONSQ", 0.0007600009777491738], ["PE incineration no Energy Recovery - CONSQ", 5.415379610194297e-06], ["PP incineration no Energy Recovery - CONSQ", 3.9979723547248786e-05], ["marginal heating grid projection updated - CONSQ", -0.00044127120437403584]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374024618735], ["autoclave - CONSQ", 0.001401066316311216], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.223466715512621e-05], ["market for polypropylene, granulate", -0.0003344346139827557], ["market for electricity, high voltage", -4.113640070802057e-05], ["transport Plastic - CONSQ", 0.0007600009777491738], ["PE incineration no Energy Recovery - CONSQ", 2.4910746218909574e-06], ["PP incineration no Energy Recovery - CONSQ", 1.8390672774610007e-05], ["marginal heating grid projection updated - CONSQ", -0.00020298475403710887]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.03862284700247247], ["alubox production - CONSQ", 0.025583158374226176], ["autoclave - CONSQ", 0.04506116156747565], ["disinfection - CONSQ", 0.049017913111261704], ["Handwash - CONSQ", 0.052961822200284316], ["alubox EoL melting - CONSQ", 0.03432235766707822], ["alubox EoL mixed sorting - CONSQ", 0.0006692049709771061], ["transport Alu - CONSQ", 0.0001377362673635314]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0754934236418704], ["autoclave - CONSQ", 0.04506116156747565], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["market for electricity, high voltage", -0.0028225081856488162], ["transport Plastic - CONSQ", 0.006012576485664547], ["PE incineration no Energy Recovery - CONSQ", 0.0005581463987091725], ["PP incineration no Energy Recovery - CONSQ", 0.004675623749452172], ["marginal heating grid projection updated - CONSQ", -0.016697884670335693]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0754934236418704], ["autoclave - CONSQ", 0.04506116156747565], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.004158278213901295], ["market for polypropylene, granulate", -0.03167408291003952], ["market for electricity, high voltage", -0.001298353765398508], ["transport Plastic - CONSQ", 0.006012576485664547], ["PE incineration no Energy Recovery - CONSQ", 0.0002567473434427218], ["PP incineration no Energy Recovery - CONSQ", 0.0021507869231092267], ["marginal heating grid projection updated - CONSQ", -0.0076810269492479585]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ.xlsx 	modified:   Brighway/Results/Ananas contribution - CONSQ.xlsx 	modified:   Brighway/Rune BE.ipynb 	modified:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/df_idx_ofir 	modified:   Brighway/life_cycle_assessment.py
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ.xlsx
+++ b/Brighway/Results/Ananas - CONSQ.xlsx
@@ -64,148 +64,148 @@
     <t>('EF v3.1 EN15804', 'water use', 'user deprivation potential (deprivation-weighted water consumption)')</t>
   </si>
   <si>
-    <t>[["alubox raw materials - CONSQ", 0.0009945931379171746], ["alubox production - CONSQ", 9.762607499157567e-05], ["autoclave - CONSQ", 0.001401428541323231], ["disinfection - CONSQ", 0.0014088446645906597], ["Handwash - CONSQ", 0.00013896582908387405], ["alubox EoL melting - CONSQ", 0.000863221102808307], ["alubox EoL mixed sorting - CONSQ", 1.3102513605718994e-05], ["transport Alu - CONSQ", 5.1128321043765874e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0009106955792616025], ["autoclave - CONSQ", 0.001401428541323231], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["market for electricity, high voltage", -0.00010747647019143262], ["transport Plastic - CONSQ", 0.0005506473682877801], ["PE incineration no Energy Recovery - CONSQ", 3.9754072547888845e-06], ["PP incineration no Energy Recovery - CONSQ", 2.9272704199409187e-05], ["marginal heating grid projection updated - CONSQ", -0.0003627581959658382]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0009106955792616025], ["autoclave - CONSQ", 0.001401428541323231], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.943299789376843e-05], ["market for polypropylene, granulate", -0.00032980866027868883], ["market for electricity, high voltage", -4.9439176288059175e-05], ["transport Plastic - CONSQ", 0.0005506473682877801], ["PE incineration no Energy Recovery - CONSQ", 1.8286873392296424e-06], ["PP incineration no Energy Recovery - CONSQ", 1.3465443823057513e-05], ["marginal heating grid projection updated - CONSQ", -0.00016686877007444426]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.15424392822864008], ["alubox production - CONSQ", 0.022156774009621943], ["autoclave - CONSQ", 0.13321320167037295], ["disinfection - CONSQ", 0.08963416459471302], ["Handwash - CONSQ", 0.02337957579346481], ["alubox EoL melting - CONSQ", 0.13106909346999387], ["alubox EoL mixed sorting - CONSQ", 0.0031809502669847747], ["transport Alu - CONSQ", 0.0021324672021639807]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.22940403947612345], ["autoclave - CONSQ", 0.13321320167037295], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["market for electricity, high voltage", -0.005961318604063036], ["transport Plastic - CONSQ", 0.060764277659934196], ["PE incineration no Energy Recovery - CONSQ", 0.03039316708934747], ["PP incineration no Energy Recovery - CONSQ", 0.2223142905005214], ["marginal heating grid projection updated - CONSQ", -0.15272040511343357]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.22940403947612345], ["autoclave - CONSQ", 0.13321320167037295], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011359305107549338], ["market for polypropylene, granulate", -0.09625534407615824], ["market for electricity, high voltage", -0.002742206557869834], ["transport Plastic - CONSQ", 0.060764277659934196], ["PE incineration no Energy Recovery - CONSQ", 0.013980856861259182], ["PP incineration no Energy Recovery - CONSQ", 0.10226457362246834], ["marginal heating grid projection updated - CONSQ", -0.0702513863552857]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.5100605935727014], ["alubox production - CONSQ", 0.11210832105151619], ["autoclave - CONSQ", 1.4495155523989065], ["disinfection - CONSQ", 1.2663943622657485], ["Handwash - CONSQ", 1.4404524083329517], ["alubox EoL melting - CONSQ", 0.24075710948842505], ["alubox EoL mixed sorting - CONSQ", 0.0175132391793385], ["transport Alu - CONSQ", 0.014308575806399947]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.6238917564937834], ["autoclave - CONSQ", 1.4495155523989065], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["market for electricity, high voltage", -0.05148097890038078], ["transport Plastic - CONSQ", 0.41868503474150837], ["PE incineration no Energy Recovery - CONSQ", 0.005492658538918375], ["PP incineration no Energy Recovery - CONSQ", 0.040469513083771405], ["marginal heating grid projection updated - CONSQ", -0.19814111293767944]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.6238917564937834], ["autoclave - CONSQ", 1.4495155523989065], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.014617415777911277], ["market for polypropylene, granulate", -0.11847606457727207], ["market for electricity, high voltage", -0.023681250294174457], ["transport Plastic - CONSQ", 0.41868503474150837], ["PE incineration no Energy Recovery - CONSQ", 0.0025266229295744123], ["PP incineration no Energy Recovery - CONSQ", 0.018615975931685874], ["marginal heating grid projection updated - CONSQ", -0.09114491198797947]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.5044803926965291], ["alubox production - CONSQ", 0.3314053978562584], ["autoclave - CONSQ", 2.6222095073851883], ["disinfection - CONSQ", 0.9614618910155737], ["Handwash - CONSQ", 0.20052001646412607], ["alubox EoL melting - CONSQ", 1.2546444967552859], ["alubox EoL mixed sorting - CONSQ", 0.03342991772325342], ["transport Alu - CONSQ", 0.03016378175125673]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 7.1063850688446575], ["autoclave - CONSQ", 2.6222095073851883], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["market for electricity, high voltage", -0.06451435176929034], ["transport Plastic - CONSQ", 0.7661470104554844], ["PE incineration no Energy Recovery - CONSQ", 0.004737511073583869], ["PP incineration no Energy Recovery - CONSQ", 0.03531591964766336], ["marginal heating grid projection updated - CONSQ", -1.9042468330459614]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 7.1063850688446575], ["autoclave - CONSQ", 2.6222095073851883], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.3917069938836761], ["market for polypropylene, granulate", -3.455013830627775], ["market for electricity, high voltage", -0.029676601813876657], ["transport Plastic - CONSQ", 0.7661470104554844], ["PE incineration no Energy Recovery - CONSQ", 0.002179255096051083], ["PP incineration no Energy Recovery - CONSQ", 0.016245322935529587], ["marginal heating grid projection updated - CONSQ", -0.8759535432763497]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.674180468862365e-05], ["alubox production - CONSQ", 1.3995384524358032e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["disinfection - CONSQ", 3.5584880575219164e-05], ["Handwash - CONSQ", 0.00018762709538521408], ["alubox EoL melting - CONSQ", 4.4898802320666606e-05], ["alubox EoL mixed sorting - CONSQ", 2.9157591258433636e-06], ["transport Alu - CONSQ", 2.1641692036306876e-07]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.6445483987961924e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["market for electricity, high voltage", -2.3521884456291384e-06], ["transport Plastic - CONSQ", 1.3662180517295428e-05], ["PE incineration no Energy Recovery - CONSQ", 4.702523210284834e-08], ["PP incineration no Energy Recovery - CONSQ", 3.7275612579358277e-07], ["marginal heating grid projection updated - CONSQ", -2.3048939664613542e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.6445483987961924e-05], ["autoclave - CONSQ", 3.44606754133238e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3834463252213407e-06], ["market for polypropylene, granulate", -1.0607017560192631e-05], ["market for electricity, high voltage", -1.0820066849895143e-06], ["transport Plastic - CONSQ", 1.3662180517295428e-05], ["PE incineration no Energy Recovery - CONSQ", 2.1631606855422463e-08], ["PP incineration no Energy Recovery - CONSQ", 1.7146781393715555e-07], ["marginal heating grid projection updated - CONSQ", -1.0602512243667338e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.000163881654485523], ["alubox production - CONSQ", 2.0912907037267336e-05], ["autoclave - CONSQ", 0.0005318438000221372], ["disinfection - CONSQ", 0.00044366254416675034], ["Handwash - CONSQ", 0.0003436229861670134], ["alubox EoL melting - CONSQ", 0.0001420371138268665], ["alubox EoL mixed sorting - CONSQ", 3.073223870126413e-06], ["transport Alu - CONSQ", 1.3826016473134355e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00020091256543071508], ["autoclave - CONSQ", 0.0005318438000221372], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["market for electricity, high voltage", -2.959148606151654e-05], ["transport Plastic - CONSQ", 0.0002401220652228008], ["PE incineration no Energy Recovery - CONSQ", 2.0429818231506584e-06], ["PP incineration no Energy Recovery - CONSQ", 1.499103348869123e-05], ["marginal heating grid projection updated - CONSQ", -0.00011074079953044283]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00020091256543071508], ["autoclave - CONSQ", 0.0005318438000221372], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.495174878614386e-06], ["market for polypropylene, granulate", -6.876059319507486e-05], ["market for electricity, high voltage", -1.3612083588297858e-05], ["transport Plastic - CONSQ", 0.0002401220652228008], ["PE incineration no Energy Recovery - CONSQ", 9.397716389335705e-07], ["PP incineration no Energy Recovery - CONSQ", 6.89587539076395e-06], ["marginal heating grid projection updated - CONSQ", -5.094076778732855e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0017368917598334101], ["alubox production - CONSQ", 0.0001856808626641268], ["autoclave - CONSQ", 0.006227844001905327], ["disinfection - CONSQ", 0.005904113186690734], ["Handwash - CONSQ", 0.00047487836259920807], ["alubox EoL melting - CONSQ", 0.0014965946551747942], ["alubox EoL mixed sorting - CONSQ", 3.0447073785008677e-05], ["transport Alu - CONSQ", 1.4256163138019514e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0021683486061642647], ["autoclave - CONSQ", 0.006227844001905327], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["market for electricity, high voltage", -0.0004665919463496633], ["transport Plastic - CONSQ", 0.00260272582979734], ["PE incineration no Energy Recovery - CONSQ", 2.0857587867818552e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0001530665074619661], ["marginal heating grid projection updated - CONSQ", -0.0012188533129356054]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0021683486061642647], ["autoclave - CONSQ", 0.006227844001905327], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.009658202656336e-05], ["market for polypropylene, granulate", -0.0007317515213936433], ["market for electricity, high voltage", -0.00021463229532084788], ["transport Plastic - CONSQ", 0.00260272582979734], ["PE incineration no Energy Recovery - CONSQ", 9.594490423206304e-06], ["PP incineration no Energy Recovery - CONSQ", 7.041059322068724e-05], ["marginal heating grid projection updated - CONSQ", -0.0005606725240835317]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 4.602823240611735e-10], ["alubox production - CONSQ", 5.309861270471534e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["disinfection - CONSQ", 3.6409678363480453e-10], ["Handwash - CONSQ", 4.322849503680417e-11], ["alubox EoL melting - CONSQ", 2.638370965941138e-10], ["alubox EoL mixed sorting - CONSQ", -1.345407722378956e-11], ["transport Alu - CONSQ", 1.1754579073721845e-12]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 8.509115427464358e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["market for electricity, high voltage", -2.5871319984405878e-11], ["transport Plastic - CONSQ", 5.3489867490061055e-11], ["PE incineration no Energy Recovery - CONSQ", 7.115851227019668e-13], ["PP incineration no Energy Recovery - CONSQ", 5.494110762407928e-12], ["marginal heating grid projection updated - CONSQ", -9.417353664137237e-11]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 8.509115427464358e-11], ["autoclave - CONSQ", 4.206479141950437e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.813968395074686e-12], ["market for polypropylene, granulate", -2.864684992177723e-11], ["market for electricity, high voltage", -1.190080719282235e-11], ["transport Plastic - CONSQ", 5.3489867490061055e-11], ["PE incineration no Energy Recovery - CONSQ", 3.273291569813087e-13], ["PP incineration no Energy Recovery - CONSQ", 2.5272909245026176e-12], ["marginal heating grid projection updated - CONSQ", -4.3319826845504436e-11]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 2.7867630139694007e-09], ["alubox production - CONSQ", 2.906200254463529e-10], ["autoclave - CONSQ", 8.116257548155443e-09], ["disinfection - CONSQ", 7.46019371490762e-09], ["Handwash - CONSQ", 1.3069723084130544e-09], ["alubox EoL melting - CONSQ", 2.029093983188106e-09], ["alubox EoL mixed sorting - CONSQ", 1.4327770049663526e-11], ["transport Alu - CONSQ", 2.203031249443254e-11]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.940653426127992e-09], ["autoclave - CONSQ", 8.116257548155443e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["market for electricity, high voltage", -5.330945378301465e-10], ["transport Plastic - CONSQ", 3.934257356952707e-10], ["PE incineration no Energy Recovery - CONSQ", 2.3717512826915464e-11], ["PP incineration no Energy Recovery - CONSQ", 1.7359564756098446e-10], ["marginal heating grid projection updated - CONSQ", -1.565397456200232e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.940653426127992e-09], ["autoclave - CONSQ", 8.116257548155443e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.698861310212956e-11], ["market for polypropylene, granulate", -6.276531983150668e-10], ["market for electricity, high voltage", -2.452234874012752e-10], ["transport Plastic - CONSQ", 3.934257356952707e-10], ["PE incineration no Energy Recovery - CONSQ", 1.0910055918006766e-11], ["PP incineration no Energy Recovery - CONSQ", 7.985399691032916e-11], ["marginal heating grid projection updated - CONSQ", -7.200828280372583e-10]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0006450722467587322], ["alubox production - CONSQ", 0.0019047788572722536], ["autoclave - CONSQ", -0.00521719640790275], ["disinfection - CONSQ", 0.000470792032781366], ["Handwash - CONSQ", 0.001755590569259854], ["alubox EoL melting - CONSQ", 0.0012467999068701253], ["alubox EoL mixed sorting - CONSQ", -0.00014755172647712224], ["transport Alu - CONSQ", 1.0961680168464363e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008495096999209003], ["autoclave - CONSQ", -0.00521719640790275], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["market for electricity, high voltage", -1.6945325686799705e-05], ["transport Plastic - CONSQ", 0.0002710560820291955], ["PE incineration no Energy Recovery - CONSQ", 3.125204459109416e-07], ["PP incineration no Energy Recovery - CONSQ", 1.7490279055748393e-06], ["marginal heating grid projection updated - CONSQ", -0.009521264122831089]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008495096999209003], ["autoclave - CONSQ", -0.00521719640790275], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00022157206170105202], ["market for polypropylene, granulate", -0.0015468389680720798], ["market for electricity, high voltage", -7.794849815918213e-06], ["transport Plastic - CONSQ", 0.0002710560820291955], ["PE incineration no Energy Recovery - CONSQ", 1.4375940582638368e-07], ["PP incineration no Energy Recovery - CONSQ", 8.045527635579575e-07], ["marginal heating grid projection updated - CONSQ", -0.004379781496367154]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.3349731984572754], ["alubox production - CONSQ", 0.3812108164908996], ["autoclave - CONSQ", 42.497287921125405], ["disinfection - CONSQ", 41.68159582891549], ["Handwash - CONSQ", 0.9278423208700517], ["alubox EoL melting - CONSQ", 0.17506952519707022], ["alubox EoL mixed sorting - CONSQ", 0.004021728747484901], ["transport Alu - CONSQ", 0.018747663837717685]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.7138591399766346], ["autoclave - CONSQ", 42.497287921125405], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["market for electricity, high voltage", -3.385238115609151], ["transport Plastic - CONSQ", 0.49202641391776436], ["PE incineration no Energy Recovery - CONSQ", -0.0005517467070879679], ["PP incineration no Energy Recovery - CONSQ", -0.003848634491936366], ["marginal heating grid projection updated - CONSQ", -4.188613614711568]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.7138591399766346], ["autoclave - CONSQ", 42.497287921125405], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.01990280748454917], ["market for polypropylene, granulate", -0.16512423556264405], ["market for electricity, high voltage", -1.5572095331801954], ["transport Plastic - CONSQ", 0.49202641391776436], ["PE incineration no Energy Recovery - CONSQ", -0.000253803430773661], ["PP incineration no Energy Recovery - CONSQ", -0.0017703723252276253], ["marginal heating grid projection updated - CONSQ", -1.9267622649850056]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.5988961824265972e-07], ["alubox production - CONSQ", 2.2129992279305888e-07], ["autoclave - CONSQ", 6.577814174539491e-06], ["disinfection - CONSQ", 6.04683667379469e-06], ["Handwash - CONSQ", 1.995155195350066e-07], ["alubox EoL melting - CONSQ", -1.001845982851653e-06], ["alubox EoL mixed sorting - CONSQ", -2.38502064057568e-07], ["transport Alu - CONSQ", 4.203508200187605e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.3437873386267166e-06], ["autoclave - CONSQ", 6.577814174539491e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["market for electricity, high voltage", -3.8494146819582574e-07], ["transport Plastic - CONSQ", -8.189405999431164e-08], ["PE incineration no Energy Recovery - CONSQ", -1.6013953846098283e-09], ["PP incineration no Energy Recovery - CONSQ", -1.300532356531317e-08], ["marginal heating grid projection updated - CONSQ", -1.6647590262392704e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.3437873386267166e-06], ["autoclave - CONSQ", 6.577814174539491e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.0160051104600511e-07], ["market for polypropylene, granulate", -8.572124772542587e-07], ["market for electricity, high voltage", -1.7707307537004648e-07], ["transport Plastic - CONSQ", -8.189405999431164e-08], ["PE incineration no Energy Recovery - CONSQ", -7.366418438366595e-10], ["PP incineration no Energy Recovery - CONSQ", -5.982450728470476e-09], ["marginal heating grid projection updated - CONSQ", -7.657891482674546e-07]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.346870114932336e-09], ["alubox production - CONSQ", 6.546061516729629e-10], ["autoclave - CONSQ", 5.322695918253996e-09], ["disinfection - CONSQ", 2.2179209318865375e-09], ["Handwash - CONSQ", 7.056252772238615e-10], ["alubox EoL melting - CONSQ", 9.80115744208019e-10], ["alubox EoL mixed sorting - CONSQ", 8.434689712810406e-11], ["transport Alu - CONSQ", 4.8640333822238504e-11]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.2672307267425193e-09], ["autoclave - CONSQ", 5.322695918253996e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["market for electricity, high voltage", -1.2104405225218283e-10], ["transport Plastic - CONSQ", 8.958388317628765e-10], ["PE incineration no Energy Recovery - CONSQ", 1.5639344084501915e-11], ["PP incineration no Energy Recovery - CONSQ", 1.1576338377537581e-10], ["marginal heating grid projection updated - CONSQ", -1.2743144554935814e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.2672307267425193e-09], ["autoclave - CONSQ", 5.322695918253996e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.1699072692562864e-10], ["market for polypropylene, granulate", -7.950858434997455e-10], ["market for electricity, high voltage", -5.568026403590827e-11], ["transport Plastic - CONSQ", 8.958388317628765e-10], ["PE incineration no Energy Recovery - CONSQ", 7.194098282618044e-12], ["PP incineration no Energy Recovery - CONSQ", 5.325115637008286e-11], ["marginal heating grid projection updated - CONSQ", -5.861846495403271e-09]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.2379513986357882e-08], ["alubox production - CONSQ", 6.17038724902976e-10], ["autoclave - CONSQ", 1.7848307122014812e-08], ["disinfection - CONSQ", 1.821998482194627e-08], ["Handwash - CONSQ", 2.1520410437413735e-09], ["alubox EoL melting - CONSQ", 1.1187702333687963e-08], ["alubox EoL mixed sorting - CONSQ", 1.9362435943939807e-10], ["transport Alu - CONSQ", 1.5196424176911972e-10]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.0430954978932512e-08], ["autoclave - CONSQ", 1.7848307122014812e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["market for electricity, high voltage", -1.4253562039393767e-09], ["transport Plastic - CONSQ", 5.884235184610808e-09], ["PE incineration no Energy Recovery - CONSQ", 1.549660557939171e-11], ["PP incineration no Energy Recovery - CONSQ", 1.3628019230621342e-10], ["marginal heating grid projection updated - CONSQ", -9.508157486501743e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.0430954978932512e-08], ["autoclave - CONSQ", 1.7848307122014812e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.747443612396433e-10], ["market for polypropylene, granulate", -4.0611447739453945e-09], ["market for electricity, high voltage", -6.55663853812118e-10], ["transport Plastic - CONSQ", 5.884235184610808e-09], ["PE incineration no Energy Recovery - CONSQ", 7.128438588213649e-12], ["PP incineration no Energy Recovery - CONSQ", 6.268888743349566e-11], ["marginal heating grid projection updated - CONSQ", -4.373752444499595e-09]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0005788419782736742], ["alubox production - CONSQ", 7.128328313713283e-05], ["autoclave - CONSQ", 0.001401066316311216], ["disinfection - CONSQ", 0.001157865918747418], ["Handwash - CONSQ", 9.142048860869044e-05], ["alubox EoL melting - CONSQ", 0.000487494665781496], ["alubox EoL mixed sorting - CONSQ", 1.7801678607102722e-05], ["transport Alu - CONSQ", 7.90076841276903e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0008421374024618735], ["autoclave - CONSQ", 0.001401066316311216], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["market for electricity, high voltage", -8.942695806091347e-05], ["transport Plastic - CONSQ", 0.0007600009777491738], ["PE incineration no Energy Recovery - CONSQ", 5.415379610194297e-06], ["PP incineration no Energy Recovery - CONSQ", 3.9979723547248786e-05], ["marginal heating grid projection updated - CONSQ", -0.00044127120437403584]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0008421374024618735], ["autoclave - CONSQ", 0.001401066316311216], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.223466715512621e-05], ["market for polypropylene, granulate", -0.0003344346139827557], ["market for electricity, high voltage", -4.113640070802057e-05], ["transport Plastic - CONSQ", 0.0007600009777491738], ["PE incineration no Energy Recovery - CONSQ", 2.4910746218909574e-06], ["PP incineration no Energy Recovery - CONSQ", 1.8390672774610007e-05], ["marginal heating grid projection updated - CONSQ", -0.00020298475403710887]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03862284700247247], ["alubox production - CONSQ", 0.025583158374226176], ["autoclave - CONSQ", 0.04506116156747565], ["disinfection - CONSQ", 0.049017913111261704], ["Handwash - CONSQ", 0.052961822200284316], ["alubox EoL melting - CONSQ", 0.03432235766707822], ["alubox EoL mixed sorting - CONSQ", 0.0006692049709771061], ["transport Alu - CONSQ", 0.0001377362673635314]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0754934236418704], ["autoclave - CONSQ", 0.04506116156747565], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["market for electricity, high voltage", -0.0028225081856488162], ["transport Plastic - CONSQ", 0.006012576485664547], ["PE incineration no Energy Recovery - CONSQ", 0.0005581463987091725], ["PP incineration no Energy Recovery - CONSQ", 0.004675623749452172], ["marginal heating grid projection updated - CONSQ", -0.016697884670335693]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0754934236418704], ["autoclave - CONSQ", 0.04506116156747565], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.004158278213901295], ["market for polypropylene, granulate", -0.03167408291003952], ["market for electricity, high voltage", -0.001298353765398508], ["transport Plastic - CONSQ", 0.006012576485664547], ["PE incineration no Energy Recovery - CONSQ", 0.0002567473434427218], ["PP incineration no Energy Recovery - CONSQ", 0.0021507869231092267], ["marginal heating grid projection updated - CONSQ", -0.0076810269492479585]]</t>
+    <t>[["alubox raw materials - CONSQ", 0.0009945931379257335], ["alubox production - CONSQ", 9.762607525302666e-05], ["autoclave - CONSQ", 0.0014014285477584704], ["Handwash - CONSQ", 0.00013896506335219004], ["alubox EoL melting - CONSQ", 0.000863221102818143], ["alubox EoL mixed sorting - CONSQ", 1.310251360070705e-05], ["transport Alu - CONSQ", 5.1128321049625e-06], ["avoided alubox raw materials - CONSQ", -0.0009303607368774412]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955793944203], ["autoclave - CONSQ", 0.0014014285477584704], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["market for electricity, high voltage", -0.00010747647019143262], ["transport Plastic - CONSQ", 0.0005506473683032066], ["PE incineration no Energy Recovery - CONSQ", -3.975407268656008e-06], ["PP incineration no Energy Recovery - CONSQ", -2.9272704022280706e-05], ["marginal heating grid projection updated - CONSQ", -0.00036275819625185637]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955793944203], ["autoclave - CONSQ", 0.0014014285477584704], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.943299789376843e-05], ["market for polypropylene, granulate", -0.00032980866027868883], ["market for electricity, high voltage", -4.9439176288059175e-05], ["transport Plastic - CONSQ", 0.0005506473683032066], ["PE incineration no Energy Recovery - CONSQ", -1.8286873438161481e-06], ["PP incineration no Energy Recovery - CONSQ", -1.3465443854649882e-05], ["marginal heating grid projection updated - CONSQ", -0.00016686877028358917]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.1542439282280466], ["alubox production - CONSQ", 0.02215677402758675], ["autoclave - CONSQ", 0.13321320196804998], ["Handwash - CONSQ", 0.023379389925914866], ["alubox EoL melting - CONSQ", 0.13106909346994217], ["alubox EoL mixed sorting - CONSQ", 0.0031809502666227257], ["transport Alu - CONSQ", 0.002132467202214205], ["avoided alubox raw materials - CONSQ", -0.1434851961767817]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.22940403948446897], ["autoclave - CONSQ", 0.13321320196804998], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["market for electricity, high voltage", -0.005961318604063036], ["transport Plastic - CONSQ", 0.06076427766020801], ["PE incineration no Energy Recovery - CONSQ", -0.030393167090429885], ["PP incineration no Energy Recovery - CONSQ", -0.22231429048713935], ["marginal heating grid projection updated - CONSQ", -0.1527204051387211]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.22940403948446897], ["autoclave - CONSQ", 0.13321320196804998], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011359305107549338], ["market for polypropylene, granulate", -0.09625534407615824], ["market for electricity, high voltage", -0.002742206557869834], ["transport Plastic - CONSQ", 0.06076427766020801], ["PE incineration no Energy Recovery - CONSQ", -0.013980856861595012], ["PP incineration no Energy Recovery - CONSQ", -0.10226457362459716], ["marginal heating grid projection updated - CONSQ", -0.07025138636451161]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.5100605935669397], ["alubox production - CONSQ", 0.1121083212752216], ["autoclave - CONSQ", 1.4495155558583146], ["Handwash - CONSQ", 1.4404517569869522], ["alubox EoL melting - CONSQ", 0.2407571094903735], ["alubox EoL mixed sorting - CONSQ", 0.017513239175206485], ["transport Alu - CONSQ", 0.014308575807010174], ["avoided alubox raw materials - CONSQ", -0.47435214475624643]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917565901918], ["autoclave - CONSQ", 1.4495155558583146], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["market for electricity, high voltage", -0.05148097890038078], ["transport Plastic - CONSQ", 0.41868503474554886], ["PE incineration no Energy Recovery - CONSQ", -0.00549265855014727], ["PP incineration no Energy Recovery - CONSQ", -0.0404695129304379], ["marginal heating grid projection updated - CONSQ", -0.19814111321719896]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917565901918], ["autoclave - CONSQ", 1.4495155558583146], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.014617415777911277], ["market for polypropylene, granulate", -0.11847606457727207], ["market for electricity, high voltage", -0.023681250294174457], ["transport Plastic - CONSQ", 0.41868503474554886], ["PE incineration no Energy Recovery - CONSQ", -0.002526622933140321], ["PP incineration no Energy Recovery - CONSQ", -0.018615975952776156], ["marginal heating grid projection updated - CONSQ", -0.09114491208579659]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.5044803926799752], ["alubox production - CONSQ", 0.33140539801010077], ["autoclave - CONSQ", 2.6222095099092844], ["Handwash - CONSQ", 0.2005184490737104], ["alubox EoL melting - CONSQ", 1.254644496749015], ["alubox EoL mixed sorting - CONSQ", 0.03342991771808647], ["transport Alu - CONSQ", 0.030163781751858625], ["avoided alubox raw materials - CONSQ", -1.3954070272327745]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.10638506894718], ["autoclave - CONSQ", 2.6222095099092844], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["market for electricity, high voltage", -0.06451435176929034], ["transport Plastic - CONSQ", 0.7661470104553016], ["PE incineration no Energy Recovery - CONSQ", -0.004737511087725779], ["PP incineration no Energy Recovery - CONSQ", -0.03531591946646204], ["marginal heating grid projection updated - CONSQ", -1.9042468334022342]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.10638506894718], ["autoclave - CONSQ", 2.6222095099092844], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.3917069938836761], ["market for polypropylene, granulate", -3.455013830627775], ["market for electricity, high voltage", -0.029676601813876657], ["transport Plastic - CONSQ", 0.7661470104553016], ["PE incineration no Energy Recovery - CONSQ", -0.002179255100414148], ["PP incineration no Energy Recovery - CONSQ", -0.016245322960517825], ["marginal heating grid projection updated - CONSQ", -0.875953543375369]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.674180468871734e-05], ["alubox production - CONSQ", 1.399538453168012e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["Handwash - CONSQ", 0.00018762705622696213], ["alubox EoL melting - CONSQ", 4.489880232077326e-05], ["alubox EoL mixed sorting - CONSQ", 2.915759125666338e-06], ["transport Alu - CONSQ", 2.164169203812253e-07], ["avoided alubox raw materials - CONSQ", -5.145297554034886e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.6445483992332553e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["market for electricity, high voltage", -2.3521884456291384e-06], ["transport Plastic - CONSQ", 1.3662180517735043e-05], ["PE incineration no Energy Recovery - CONSQ", -4.702523270879441e-08], ["PP incineration no Energy Recovery - CONSQ", -3.7275611977706703e-07], ["marginal heating grid projection updated - CONSQ", -2.304893967580168e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.6445483992332553e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3834463252213407e-06], ["market for polypropylene, granulate", -1.0607017560192631e-05], ["market for electricity, high voltage", -1.0820066849895143e-06], ["transport Plastic - CONSQ", 1.3662180517735043e-05], ["PE incineration no Energy Recovery - CONSQ", -2.163160704158951e-08], ["PP incineration no Energy Recovery - CONSQ", -1.7146781536286209e-07], ["marginal heating grid projection updated - CONSQ", -1.0602512251197134e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00016388165448494917], ["alubox production - CONSQ", 2.0912907070932413e-05], ["autoclave - CONSQ", 0.0005318438005531931], ["Handwash - CONSQ", 0.0003436227578841364], ["alubox EoL melting - CONSQ", 0.00014203711382730026], ["alubox EoL mixed sorting - CONSQ", 3.0732238694586672e-06], ["transport Alu - CONSQ", 1.3826016473976873e-06], ["avoided alubox raw materials - CONSQ", -0.00015291400012868402]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256544607316], ["autoclave - CONSQ", 0.0005318438005531931], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["market for electricity, high voltage", -2.959148606151654e-05], ["transport Plastic - CONSQ", 0.0002401220652235828], ["PE incineration no Energy Recovery - CONSQ", -2.042981824985719e-06], ["PP incineration no Energy Recovery - CONSQ", -1.4991033464379707e-05], ["marginal heating grid projection updated - CONSQ", -0.00011074079957546867]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256544607316], ["autoclave - CONSQ", 0.0005318438005531931], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.495174878614386e-06], ["market for polypropylene, granulate", -6.876059319507486e-05], ["market for electricity, high voltage", -1.3612083588297858e-05], ["transport Plastic - CONSQ", 0.0002401220652235828], ["PE incineration no Energy Recovery - CONSQ", -9.397716395135968e-07], ["PP incineration no Energy Recovery - CONSQ", -6.895875394324011e-06], ["marginal heating grid projection updated - CONSQ", -5.094076780552843e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0017368917598131175], ["alubox production - CONSQ", 0.00018568086326642397], ["autoclave - CONSQ", 0.006227844010437098], ["Handwash - CONSQ", 0.0004748759142791099], ["alubox EoL melting - CONSQ", 0.0014965946551786834], ["alubox EoL mixed sorting - CONSQ", 3.0447073775253588e-05], ["transport Alu - CONSQ", 1.4256163139730771e-05], ["avoided alubox raw materials - CONSQ", -0.0016204289390099815]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486063990335], ["autoclave - CONSQ", 0.006227844010437098], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["market for electricity, high voltage", -0.0004665919463496633], ["transport Plastic - CONSQ", 0.0026027258298035906], ["PE incineration no Energy Recovery - CONSQ", -2.0857587893567897e-05], ["PP incineration no Energy Recovery - CONSQ", -0.00015306650707638396], ["marginal heating grid projection updated - CONSQ", -0.0012188533136151271]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486063990335], ["autoclave - CONSQ", 0.006227844010437098], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.009658202656336e-05], ["market for polypropylene, granulate", -0.0007317515213936433], ["market for electricity, high voltage", -0.00021463229532084788], ["transport Plastic - CONSQ", 0.0026027258298035906], ["PE incineration no Energy Recovery - CONSQ", -9.594490431244823e-06], ["PP incineration no Energy Recovery - CONSQ", -7.04105932671943e-05], ["marginal heating grid projection updated - CONSQ", -0.0005606725242770091]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.6028232405921916e-10], ["alubox production - CONSQ", 5.309861276059754e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["Handwash - CONSQ", 4.322801613089766e-11], ["alubox EoL melting - CONSQ", 2.638370965986997e-10], ["alubox EoL mixed sorting - CONSQ", -1.3454077224767679e-11], ["transport Alu - CONSQ", 1.1754579075184077e-12], ["avoided alubox raw materials - CONSQ", -3.874427537424086e-10]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115433817886e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["market for electricity, high voltage", -2.5871319984405878e-11], ["transport Plastic - CONSQ", 5.348986749143977e-11], ["PE incineration no Energy Recovery - CONSQ", -7.115851265249747e-13], ["PP incineration no Energy Recovery - CONSQ", -5.4941107196955855e-12], ["marginal heating grid projection updated - CONSQ", -9.417353671792283e-11]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115433817886e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.813968395074686e-12], ["market for polypropylene, granulate", -2.864684992177723e-11], ["market for electricity, high voltage", -1.190080719282235e-11], ["transport Plastic - CONSQ", 5.348986749143977e-11], ["PE incineration no Energy Recovery - CONSQ", -3.2732915816765427e-13], ["PP incineration no Energy Recovery - CONSQ", -2.5272909329057136e-12], ["marginal heating grid projection updated - CONSQ", -4.331982689266619e-11]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.7867630139665452e-09], ["alubox production - CONSQ", 2.9062002769646526e-10], ["autoclave - CONSQ", 8.116257614104312e-09], ["Handwash - CONSQ", 1.3069705508780732e-09], ["alubox EoL melting - CONSQ", 2.0290939838565286e-09], ["alubox EoL mixed sorting - CONSQ", 1.432777002730035e-11], ["transport Alu - CONSQ", 2.2030312497603955e-11], ["avoided alubox raw materials - CONSQ", -2.610198125589187e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.940653431392336e-09], ["autoclave - CONSQ", 8.116257614104312e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["market for electricity, high voltage", -5.330945378301465e-10], ["transport Plastic - CONSQ", 3.934257358112044e-10], ["PE incineration no Energy Recovery - CONSQ", -2.3717512952286525e-11], ["PP incineration no Energy Recovery - CONSQ", -1.735956461646673e-10], ["marginal heating grid projection updated - CONSQ", -1.5653974582208452e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.940653431392336e-09], ["autoclave - CONSQ", 8.116257614104312e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.698861310212956e-11], ["market for polypropylene, granulate", -6.276531983150668e-10], ["market for electricity, high voltage", -2.452234874012752e-10], ["transport Plastic - CONSQ", 3.934257358112044e-10], ["PE incineration no Energy Recovery - CONSQ", -1.0910055962622929e-11], ["PP incineration no Energy Recovery - CONSQ", -7.985399724540797e-11], ["marginal heating grid projection updated - CONSQ", -7.200828307956157e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0006450722469990166], ["alubox production - CONSQ", 0.0019047788542248623], ["autoclave - CONSQ", -0.005217196391827695], ["Handwash - CONSQ", 0.0017555824933608323], ["alubox EoL melting - CONSQ", 0.001246799906905342], ["alubox EoL mixed sorting - CONSQ", -0.00014755172649235802], ["transport Alu - CONSQ", 1.0961680171087408e-05], ["avoided alubox raw materials - CONSQ", -0.0006998236723210765]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999780918], ["autoclave - CONSQ", -0.005217196391827695], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["market for electricity, high voltage", -1.6945325686799705e-05], ["transport Plastic - CONSQ", 0.0002710560820651073], ["PE incineration no Energy Recovery - CONSQ", -3.125204433518376e-07], ["PP incineration no Energy Recovery - CONSQ", -1.7490279476974062e-06], ["marginal heating grid projection updated - CONSQ", -0.009521264122772906]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999780918], ["autoclave - CONSQ", -0.005217196391827695], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00022157206170105202], ["market for polypropylene, granulate", -0.0015468389680720798], ["market for electricity, high voltage", -7.794849815918213e-06], ["transport Plastic - CONSQ", 0.0002710560820651073], ["PE incineration no Energy Recovery - CONSQ", -1.4375941444337215e-07], ["PP incineration no Energy Recovery - CONSQ", -8.045527598037418e-07], ["marginal heating grid projection updated - CONSQ", -0.004379781496595885]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.3349731985928215], ["alubox production - CONSQ", 0.3812108199860487], ["autoclave - CONSQ", 42.497287939648714], ["Handwash - CONSQ", 0.9278417141311122], ["alubox EoL melting - CONSQ", 0.17506952539415502], ["alubox EoL mixed sorting - CONSQ", 0.004021728720546831], ["transport Alu - CONSQ", 0.018747663840123607], ["avoided alubox raw materials - CONSQ", -0.2838220781200499]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591403521451], ["autoclave - CONSQ", 42.497287939648714], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["market for electricity, high voltage", -3.385238115609151], ["transport Plastic - CONSQ", 0.49202641383908585], ["PE incineration no Energy Recovery - CONSQ", 0.0005517466329439449], ["PP incineration no Energy Recovery - CONSQ", 0.003848634847957056], ["marginal heating grid projection updated - CONSQ", -4.188613611840945]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591403521451], ["autoclave - CONSQ", 42.497287939648714], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.01990280748454917], ["market for polypropylene, granulate", -0.16512423556264405], ["market for electricity, high voltage", -1.5572095331801954], ["transport Plastic - CONSQ", 0.49202641383908585], ["PE incineration no Energy Recovery - CONSQ", 0.0002538034533408767], ["PP incineration no Energy Recovery - CONSQ", 0.0017703720072125729], ["marginal heating grid projection updated - CONSQ", -1.926762261447604]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.598896187344793e-07], ["alubox production - CONSQ", 2.212999268910459e-07], ["autoclave - CONSQ", 6.577814325168771e-06], ["Handwash - CONSQ", 1.9951474886944844e-07], ["alubox EoL melting - CONSQ", -1.0018459824575312e-06], ["alubox EoL mixed sorting - CONSQ", -2.3850206414910114e-07], ["transport Alu - CONSQ", 4.203508205346124e-09], ["avoided alubox raw materials - CONSQ", -1.4329149774885112e-07]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.34378734115991e-06], ["autoclave - CONSQ", 6.577814325168771e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["market for electricity, high voltage", -3.8494146819582574e-07], ["transport Plastic - CONSQ", -8.189405946314385e-08], ["PE incineration no Energy Recovery - CONSQ", 1.601395143993557e-09], ["PP incineration no Energy Recovery - CONSQ", 1.3005326283094658e-08], ["marginal heating grid projection updated - CONSQ", -1.6647590302043975e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.34378734115991e-06], ["autoclave - CONSQ", 6.577814325168771e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.0160051104600511e-07], ["market for polypropylene, granulate", -8.572124772542587e-07], ["market for electricity, high voltage", -1.7707307537004648e-07], ["transport Plastic - CONSQ", -8.189405946314385e-08], ["PE incineration no Energy Recovery - CONSQ", 7.366417576088244e-10], ["PP incineration no Energy Recovery - CONSQ", 5.982450059514068e-09], ["marginal heating grid projection updated - CONSQ", -7.657891539247242e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.3468701148912575e-09], ["alubox production - CONSQ", 6.546061520022523e-10], ["autoclave - CONSQ", 5.322695922815759e-09], ["Handwash - CONSQ", 7.056236692456607e-10], ["alubox EoL melting - CONSQ", 9.80115744176637e-10], ["alubox EoL mixed sorting - CONSQ", 8.434689712027004e-11], ["transport Alu - CONSQ", 4.8640333823483313e-11], ["avoided alubox raw materials - CONSQ", -1.2225472022695042e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.2672307267960015e-09], ["autoclave - CONSQ", 5.322695922815759e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["market for electricity, high voltage", -1.2104405225218283e-10], ["transport Plastic - CONSQ", 8.958388317621908e-10], ["PE incineration no Energy Recovery - CONSQ", -1.563934410800861e-11], ["PP incineration no Energy Recovery - CONSQ", -1.1576338348392322e-10], ["marginal heating grid projection updated - CONSQ", -1.2743144555507371e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.2672307267960015e-09], ["autoclave - CONSQ", 5.322695922815759e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.1699072692562864e-10], ["market for polypropylene, granulate", -7.950858434997455e-10], ["market for electricity, high voltage", -5.568026403590827e-11], ["transport Plastic - CONSQ", 8.958388317621908e-10], ["PE incineration no Energy Recovery - CONSQ", -7.194098289578784e-12], ["PP incineration no Energy Recovery - CONSQ", -5.325115641365981e-11], ["marginal heating grid projection updated - CONSQ", -5.861846495549252e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.2379513986258826e-08], ["alubox production - CONSQ", 6.170387277465736e-10], ["autoclave - CONSQ", 1.7848307157297192e-08], ["Handwash - CONSQ", 2.1520213327406356e-09], ["alubox EoL melting - CONSQ", 1.11877023336995e-08], ["alubox EoL mixed sorting - CONSQ", 1.936243593958415e-10], ["transport Alu - CONSQ", 1.5196424177717214e-10], ["avoided alubox raw materials - CONSQ", -1.1638319464952641e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.0430954980012049e-08], ["autoclave - CONSQ", 1.7848307157297192e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["market for electricity, high voltage", -1.4253562039393767e-09], ["transport Plastic - CONSQ", 5.88423518461901e-09], ["PE incineration no Energy Recovery - CONSQ", -1.5496605705058103e-11], ["PP incineration no Energy Recovery - CONSQ", -1.3628019043453102e-10], ["marginal heating grid projection updated - CONSQ", -9.508157489743055e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.0430954980012049e-08], ["autoclave - CONSQ", 1.7848307157297192e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.747443612396433e-10], ["market for polypropylene, granulate", -4.0611447739453945e-09], ["market for electricity, high voltage", -6.55663853812118e-10], ["transport Plastic - CONSQ", 5.88423518461901e-09], ["PE incineration no Energy Recovery - CONSQ", -7.128438624962499e-12], ["PP incineration no Energy Recovery - CONSQ", -6.26888876612392e-11], ["marginal heating grid projection updated - CONSQ", -4.3737524453639915e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005788419782701951], ["alubox production - CONSQ", 7.128328326307099e-05], ["autoclave - CONSQ", 0.0014010663180142027], ["Handwash - CONSQ", 9.14197251274628e-05], ["alubox EoL melting - CONSQ", 0.0004874946657819522], ["alubox EoL mixed sorting - CONSQ", 1.780167860430808e-05], ["transport Alu - CONSQ", 7.900768413078576e-06], ["avoided alubox raw materials - CONSQ", -0.0005375470665861999]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374025219222], ["autoclave - CONSQ", 0.0014010663180142027], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["market for electricity, high voltage", -8.942695806091347e-05], ["transport Plastic - CONSQ", 0.0007600009777508464], ["PE incineration no Energy Recovery - CONSQ", -5.415379617993103e-06], ["PP incineration no Energy Recovery - CONSQ", -3.997972344788057e-05], ["marginal heating grid projection updated - CONSQ", -0.0004412712045675308]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374025219222], ["autoclave - CONSQ", 0.0014010663180142027], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.223466715512621e-05], ["market for polypropylene, granulate", -0.0003344346139827557], ["market for electricity, high voltage", -4.113640070802057e-05], ["transport Plastic - CONSQ", 0.0007600009777508464], ["PE incineration no Energy Recovery - CONSQ", -2.491074624346275e-06], ["PP incineration no Energy Recovery - CONSQ", -1.8390672788989974e-05], ["marginal heating grid projection updated - CONSQ", -0.00020298475410504232]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.03862284700230107], ["alubox production - CONSQ", 0.025583158377687723], ["autoclave - CONSQ", 0.04506116162085487], ["Handwash - CONSQ", 0.052961791147733764], ["alubox EoL melting - CONSQ", 0.034322357667014906], ["alubox EoL mixed sorting - CONSQ", 0.0006692049709012063], ["transport Alu - CONSQ", 0.00013773626737402736], ["avoided alubox raw materials - CONSQ", -0.03594166704133421]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.07549342364357263], ["autoclave - CONSQ", 0.04506116162085487], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["market for electricity, high voltage", -0.0028225081856488162], ["transport Plastic - CONSQ", 0.006012576485682125], ["PE incineration no Energy Recovery - CONSQ", -0.0005581463989573615], ["PP incineration no Energy Recovery - CONSQ", -0.004675623746658543], ["marginal heating grid projection updated - CONSQ", -0.016697884675900988]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.07549342364357263], ["autoclave - CONSQ", 0.04506116162085487], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.004158278213901295], ["market for polypropylene, granulate", -0.03167408291003952], ["market for electricity, high voltage", -0.001298353765398508], ["transport Plastic - CONSQ", 0.006012576485682125], ["PE incineration no Energy Recovery - CONSQ", -0.0002567473435168879], ["PP incineration no Energy Recovery - CONSQ", -0.0021507869235897125], ["marginal heating grid projection updated - CONSQ", -0.007681026951084412]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ.xlsx 	modified:   Brighway/Results/Ananas contribution - CONSQ.xlsx 	modified:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ.xlsx
+++ b/Brighway/Results/Ananas - CONSQ.xlsx
@@ -64,148 +64,148 @@
     <t>('EF v3.1 EN15804', 'water use', 'user deprivation potential (deprivation-weighted water consumption)')</t>
   </si>
   <si>
-    <t>[["alubox raw materials - CONSQ", 0.0009945931379257335], ["alubox production - CONSQ", 9.762607525302666e-05], ["autoclave - CONSQ", 0.0014014285477584704], ["Handwash - CONSQ", 0.00013896506335219004], ["alubox EoL melting - CONSQ", 0.000863221102818143], ["alubox EoL mixed sorting - CONSQ", 1.310251360070705e-05], ["transport Alu - CONSQ", 5.1128321049625e-06], ["avoided alubox raw materials - CONSQ", -0.0009303607368774412]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0009106955793944203], ["autoclave - CONSQ", 0.0014014285477584704], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["market for electricity, high voltage", -0.00010747647019143262], ["transport Plastic - CONSQ", 0.0005506473683032066], ["PE incineration no Energy Recovery - CONSQ", -3.975407268656008e-06], ["PP incineration no Energy Recovery - CONSQ", -2.9272704022280706e-05], ["marginal heating grid projection updated - CONSQ", -0.00036275819625185637]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0009106955793944203], ["autoclave - CONSQ", 0.0014014285477584704], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.943299789376843e-05], ["market for polypropylene, granulate", -0.00032980866027868883], ["market for electricity, high voltage", -4.9439176288059175e-05], ["transport Plastic - CONSQ", 0.0005506473683032066], ["PE incineration no Energy Recovery - CONSQ", -1.8286873438161481e-06], ["PP incineration no Energy Recovery - CONSQ", -1.3465443854649882e-05], ["marginal heating grid projection updated - CONSQ", -0.00016686877028358917]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.1542439282280466], ["alubox production - CONSQ", 0.02215677402758675], ["autoclave - CONSQ", 0.13321320196804998], ["Handwash - CONSQ", 0.023379389925914866], ["alubox EoL melting - CONSQ", 0.13106909346994217], ["alubox EoL mixed sorting - CONSQ", 0.0031809502666227257], ["transport Alu - CONSQ", 0.002132467202214205], ["avoided alubox raw materials - CONSQ", -0.1434851961767817]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.22940403948446897], ["autoclave - CONSQ", 0.13321320196804998], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["market for electricity, high voltage", -0.005961318604063036], ["transport Plastic - CONSQ", 0.06076427766020801], ["PE incineration no Energy Recovery - CONSQ", -0.030393167090429885], ["PP incineration no Energy Recovery - CONSQ", -0.22231429048713935], ["marginal heating grid projection updated - CONSQ", -0.1527204051387211]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.22940403948446897], ["autoclave - CONSQ", 0.13321320196804998], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011359305107549338], ["market for polypropylene, granulate", -0.09625534407615824], ["market for electricity, high voltage", -0.002742206557869834], ["transport Plastic - CONSQ", 0.06076427766020801], ["PE incineration no Energy Recovery - CONSQ", -0.013980856861595012], ["PP incineration no Energy Recovery - CONSQ", -0.10226457362459716], ["marginal heating grid projection updated - CONSQ", -0.07025138636451161]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.5100605935669397], ["alubox production - CONSQ", 0.1121083212752216], ["autoclave - CONSQ", 1.4495155558583146], ["Handwash - CONSQ", 1.4404517569869522], ["alubox EoL melting - CONSQ", 0.2407571094903735], ["alubox EoL mixed sorting - CONSQ", 0.017513239175206485], ["transport Alu - CONSQ", 0.014308575807010174], ["avoided alubox raw materials - CONSQ", -0.47435214475624643]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.6238917565901918], ["autoclave - CONSQ", 1.4495155558583146], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["market for electricity, high voltage", -0.05148097890038078], ["transport Plastic - CONSQ", 0.41868503474554886], ["PE incineration no Energy Recovery - CONSQ", -0.00549265855014727], ["PP incineration no Energy Recovery - CONSQ", -0.0404695129304379], ["marginal heating grid projection updated - CONSQ", -0.19814111321719896]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.6238917565901918], ["autoclave - CONSQ", 1.4495155558583146], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.014617415777911277], ["market for polypropylene, granulate", -0.11847606457727207], ["market for electricity, high voltage", -0.023681250294174457], ["transport Plastic - CONSQ", 0.41868503474554886], ["PE incineration no Energy Recovery - CONSQ", -0.002526622933140321], ["PP incineration no Energy Recovery - CONSQ", -0.018615975952776156], ["marginal heating grid projection updated - CONSQ", -0.09114491208579659]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.5044803926799752], ["alubox production - CONSQ", 0.33140539801010077], ["autoclave - CONSQ", 2.6222095099092844], ["Handwash - CONSQ", 0.2005184490737104], ["alubox EoL melting - CONSQ", 1.254644496749015], ["alubox EoL mixed sorting - CONSQ", 0.03342991771808647], ["transport Alu - CONSQ", 0.030163781751858625], ["avoided alubox raw materials - CONSQ", -1.3954070272327745]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 7.10638506894718], ["autoclave - CONSQ", 2.6222095099092844], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["market for electricity, high voltage", -0.06451435176929034], ["transport Plastic - CONSQ", 0.7661470104553016], ["PE incineration no Energy Recovery - CONSQ", -0.004737511087725779], ["PP incineration no Energy Recovery - CONSQ", -0.03531591946646204], ["marginal heating grid projection updated - CONSQ", -1.9042468334022342]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 7.10638506894718], ["autoclave - CONSQ", 2.6222095099092844], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.3917069938836761], ["market for polypropylene, granulate", -3.455013830627775], ["market for electricity, high voltage", -0.029676601813876657], ["transport Plastic - CONSQ", 0.7661470104553016], ["PE incineration no Energy Recovery - CONSQ", -0.002179255100414148], ["PP incineration no Energy Recovery - CONSQ", -0.016245322960517825], ["marginal heating grid projection updated - CONSQ", -0.875953543375369]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.674180468871734e-05], ["alubox production - CONSQ", 1.399538453168012e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["Handwash - CONSQ", 0.00018762705622696213], ["alubox EoL melting - CONSQ", 4.489880232077326e-05], ["alubox EoL mixed sorting - CONSQ", 2.915759125666338e-06], ["transport Alu - CONSQ", 2.164169203812253e-07], ["avoided alubox raw materials - CONSQ", -5.145297554034886e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.6445483992332553e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["market for electricity, high voltage", -2.3521884456291384e-06], ["transport Plastic - CONSQ", 1.3662180517735043e-05], ["PE incineration no Energy Recovery - CONSQ", -4.702523270879441e-08], ["PP incineration no Energy Recovery - CONSQ", -3.7275611977706703e-07], ["marginal heating grid projection updated - CONSQ", -2.304893967580168e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.6445483992332553e-05], ["autoclave - CONSQ", 3.4460675603400636e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3834463252213407e-06], ["market for polypropylene, granulate", -1.0607017560192631e-05], ["market for electricity, high voltage", -1.0820066849895143e-06], ["transport Plastic - CONSQ", 1.3662180517735043e-05], ["PE incineration no Energy Recovery - CONSQ", -2.163160704158951e-08], ["PP incineration no Energy Recovery - CONSQ", -1.7146781536286209e-07], ["marginal heating grid projection updated - CONSQ", -1.0602512251197134e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.00016388165448494917], ["alubox production - CONSQ", 2.0912907070932413e-05], ["autoclave - CONSQ", 0.0005318438005531931], ["Handwash - CONSQ", 0.0003436227578841364], ["alubox EoL melting - CONSQ", 0.00014203711382730026], ["alubox EoL mixed sorting - CONSQ", 3.0732238694586672e-06], ["transport Alu - CONSQ", 1.3826016473976873e-06], ["avoided alubox raw materials - CONSQ", -0.00015291400012868402]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00020091256544607316], ["autoclave - CONSQ", 0.0005318438005531931], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["market for electricity, high voltage", -2.959148606151654e-05], ["transport Plastic - CONSQ", 0.0002401220652235828], ["PE incineration no Energy Recovery - CONSQ", -2.042981824985719e-06], ["PP incineration no Energy Recovery - CONSQ", -1.4991033464379707e-05], ["marginal heating grid projection updated - CONSQ", -0.00011074079957546867]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00020091256544607316], ["autoclave - CONSQ", 0.0005318438005531931], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.495174878614386e-06], ["market for polypropylene, granulate", -6.876059319507486e-05], ["market for electricity, high voltage", -1.3612083588297858e-05], ["transport Plastic - CONSQ", 0.0002401220652235828], ["PE incineration no Energy Recovery - CONSQ", -9.397716395135968e-07], ["PP incineration no Energy Recovery - CONSQ", -6.895875394324011e-06], ["marginal heating grid projection updated - CONSQ", -5.094076780552843e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0017368917598131175], ["alubox production - CONSQ", 0.00018568086326642397], ["autoclave - CONSQ", 0.006227844010437098], ["Handwash - CONSQ", 0.0004748759142791099], ["alubox EoL melting - CONSQ", 0.0014965946551786834], ["alubox EoL mixed sorting - CONSQ", 3.0447073775253588e-05], ["transport Alu - CONSQ", 1.4256163139730771e-05], ["avoided alubox raw materials - CONSQ", -0.0016204289390099815]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0021683486063990335], ["autoclave - CONSQ", 0.006227844010437098], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["market for electricity, high voltage", -0.0004665919463496633], ["transport Plastic - CONSQ", 0.0026027258298035906], ["PE incineration no Energy Recovery - CONSQ", -2.0857587893567897e-05], ["PP incineration no Energy Recovery - CONSQ", -0.00015306650707638396], ["marginal heating grid projection updated - CONSQ", -0.0012188533136151271]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0021683486063990335], ["autoclave - CONSQ", 0.006227844010437098], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.009658202656336e-05], ["market for polypropylene, granulate", -0.0007317515213936433], ["market for electricity, high voltage", -0.00021463229532084788], ["transport Plastic - CONSQ", 0.0026027258298035906], ["PE incineration no Energy Recovery - CONSQ", -9.594490431244823e-06], ["PP incineration no Energy Recovery - CONSQ", -7.04105932671943e-05], ["marginal heating grid projection updated - CONSQ", -0.0005606725242770091]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 4.6028232405921916e-10], ["alubox production - CONSQ", 5.309861276059754e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["Handwash - CONSQ", 4.322801613089766e-11], ["alubox EoL melting - CONSQ", 2.638370965986997e-10], ["alubox EoL mixed sorting - CONSQ", -1.3454077224767679e-11], ["transport Alu - CONSQ", 1.1754579075184077e-12], ["avoided alubox raw materials - CONSQ", -3.874427537424086e-10]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 8.509115433817886e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["market for electricity, high voltage", -2.5871319984405878e-11], ["transport Plastic - CONSQ", 5.348986749143977e-11], ["PE incineration no Energy Recovery - CONSQ", -7.115851265249747e-13], ["PP incineration no Energy Recovery - CONSQ", -5.4941107196955855e-12], ["marginal heating grid projection updated - CONSQ", -9.417353671792283e-11]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 8.509115433817886e-11], ["autoclave - CONSQ", 4.206479154205136e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.813968395074686e-12], ["market for polypropylene, granulate", -2.864684992177723e-11], ["market for electricity, high voltage", -1.190080719282235e-11], ["transport Plastic - CONSQ", 5.348986749143977e-11], ["PE incineration no Energy Recovery - CONSQ", -3.2732915816765427e-13], ["PP incineration no Energy Recovery - CONSQ", -2.5272909329057136e-12], ["marginal heating grid projection updated - CONSQ", -4.331982689266619e-11]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 2.7867630139665452e-09], ["alubox production - CONSQ", 2.9062002769646526e-10], ["autoclave - CONSQ", 8.116257614104312e-09], ["Handwash - CONSQ", 1.3069705508780732e-09], ["alubox EoL melting - CONSQ", 2.0290939838565286e-09], ["alubox EoL mixed sorting - CONSQ", 1.432777002730035e-11], ["transport Alu - CONSQ", 2.2030312497603955e-11], ["avoided alubox raw materials - CONSQ", -2.610198125589187e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.940653431392336e-09], ["autoclave - CONSQ", 8.116257614104312e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["market for electricity, high voltage", -5.330945378301465e-10], ["transport Plastic - CONSQ", 3.934257358112044e-10], ["PE incineration no Energy Recovery - CONSQ", -2.3717512952286525e-11], ["PP incineration no Energy Recovery - CONSQ", -1.735956461646673e-10], ["marginal heating grid projection updated - CONSQ", -1.5653974582208452e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.940653431392336e-09], ["autoclave - CONSQ", 8.116257614104312e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.698861310212956e-11], ["market for polypropylene, granulate", -6.276531983150668e-10], ["market for electricity, high voltage", -2.452234874012752e-10], ["transport Plastic - CONSQ", 3.934257358112044e-10], ["PE incineration no Energy Recovery - CONSQ", -1.0910055962622929e-11], ["PP incineration no Energy Recovery - CONSQ", -7.985399724540797e-11], ["marginal heating grid projection updated - CONSQ", -7.200828307956157e-10]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0006450722469990166], ["alubox production - CONSQ", 0.0019047788542248623], ["autoclave - CONSQ", -0.005217196391827695], ["Handwash - CONSQ", 0.0017555824933608323], ["alubox EoL melting - CONSQ", 0.001246799906905342], ["alubox EoL mixed sorting - CONSQ", -0.00014755172649235802], ["transport Alu - CONSQ", 1.0961680171087408e-05], ["avoided alubox raw materials - CONSQ", -0.0006998236723210765]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008495096999780918], ["autoclave - CONSQ", -0.005217196391827695], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["market for electricity, high voltage", -1.6945325686799705e-05], ["transport Plastic - CONSQ", 0.0002710560820651073], ["PE incineration no Energy Recovery - CONSQ", -3.125204433518376e-07], ["PP incineration no Energy Recovery - CONSQ", -1.7490279476974062e-06], ["marginal heating grid projection updated - CONSQ", -0.009521264122772906]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008495096999780918], ["autoclave - CONSQ", -0.005217196391827695], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00022157206170105202], ["market for polypropylene, granulate", -0.0015468389680720798], ["market for electricity, high voltage", -7.794849815918213e-06], ["transport Plastic - CONSQ", 0.0002710560820651073], ["PE incineration no Energy Recovery - CONSQ", -1.4375941444337215e-07], ["PP incineration no Energy Recovery - CONSQ", -8.045527598037418e-07], ["marginal heating grid projection updated - CONSQ", -0.004379781496595885]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.3349731985928215], ["alubox production - CONSQ", 0.3812108199860487], ["autoclave - CONSQ", 42.497287939648714], ["Handwash - CONSQ", 0.9278417141311122], ["alubox EoL melting - CONSQ", 0.17506952539415502], ["alubox EoL mixed sorting - CONSQ", 0.004021728720546831], ["transport Alu - CONSQ", 0.018747663840123607], ["avoided alubox raw materials - CONSQ", -0.2838220781200499]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.7138591403521451], ["autoclave - CONSQ", 42.497287939648714], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["market for electricity, high voltage", -3.385238115609151], ["transport Plastic - CONSQ", 0.49202641383908585], ["PE incineration no Energy Recovery - CONSQ", 0.0005517466329439449], ["PP incineration no Energy Recovery - CONSQ", 0.003848634847957056], ["marginal heating grid projection updated - CONSQ", -4.188613611840945]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.7138591403521451], ["autoclave - CONSQ", 42.497287939648714], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.01990280748454917], ["market for polypropylene, granulate", -0.16512423556264405], ["market for electricity, high voltage", -1.5572095331801954], ["transport Plastic - CONSQ", 0.49202641383908585], ["PE incineration no Energy Recovery - CONSQ", 0.0002538034533408767], ["PP incineration no Energy Recovery - CONSQ", 0.0017703720072125729], ["marginal heating grid projection updated - CONSQ", -1.926762261447604]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.598896187344793e-07], ["alubox production - CONSQ", 2.212999268910459e-07], ["autoclave - CONSQ", 6.577814325168771e-06], ["Handwash - CONSQ", 1.9951474886944844e-07], ["alubox EoL melting - CONSQ", -1.0018459824575312e-06], ["alubox EoL mixed sorting - CONSQ", -2.3850206414910114e-07], ["transport Alu - CONSQ", 4.203508205346124e-09], ["avoided alubox raw materials - CONSQ", -1.4329149774885112e-07]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.34378734115991e-06], ["autoclave - CONSQ", 6.577814325168771e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["market for electricity, high voltage", -3.8494146819582574e-07], ["transport Plastic - CONSQ", -8.189405946314385e-08], ["PE incineration no Energy Recovery - CONSQ", 1.601395143993557e-09], ["PP incineration no Energy Recovery - CONSQ", 1.3005326283094658e-08], ["marginal heating grid projection updated - CONSQ", -1.6647590302043975e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.34378734115991e-06], ["autoclave - CONSQ", 6.577814325168771e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.0160051104600511e-07], ["market for polypropylene, granulate", -8.572124772542587e-07], ["market for electricity, high voltage", -1.7707307537004648e-07], ["transport Plastic - CONSQ", -8.189405946314385e-08], ["PE incineration no Energy Recovery - CONSQ", 7.366417576088244e-10], ["PP incineration no Energy Recovery - CONSQ", 5.982450059514068e-09], ["marginal heating grid projection updated - CONSQ", -7.657891539247242e-07]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.3468701148912575e-09], ["alubox production - CONSQ", 6.546061520022523e-10], ["autoclave - CONSQ", 5.322695922815759e-09], ["Handwash - CONSQ", 7.056236692456607e-10], ["alubox EoL melting - CONSQ", 9.80115744176637e-10], ["alubox EoL mixed sorting - CONSQ", 8.434689712027004e-11], ["transport Alu - CONSQ", 4.8640333823483313e-11], ["avoided alubox raw materials - CONSQ", -1.2225472022695042e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.2672307267960015e-09], ["autoclave - CONSQ", 5.322695922815759e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["market for electricity, high voltage", -1.2104405225218283e-10], ["transport Plastic - CONSQ", 8.958388317621908e-10], ["PE incineration no Energy Recovery - CONSQ", -1.563934410800861e-11], ["PP incineration no Energy Recovery - CONSQ", -1.1576338348392322e-10], ["marginal heating grid projection updated - CONSQ", -1.2743144555507371e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 2.2672307267960015e-09], ["autoclave - CONSQ", 5.322695922815759e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.1699072692562864e-10], ["market for polypropylene, granulate", -7.950858434997455e-10], ["market for electricity, high voltage", -5.568026403590827e-11], ["transport Plastic - CONSQ", 8.958388317621908e-10], ["PE incineration no Energy Recovery - CONSQ", -7.194098289578784e-12], ["PP incineration no Energy Recovery - CONSQ", -5.325115641365981e-11], ["marginal heating grid projection updated - CONSQ", -5.861846495549252e-09]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 1.2379513986258826e-08], ["alubox production - CONSQ", 6.170387277465736e-10], ["autoclave - CONSQ", 1.7848307157297192e-08], ["Handwash - CONSQ", 2.1520213327406356e-09], ["alubox EoL melting - CONSQ", 1.11877023336995e-08], ["alubox EoL mixed sorting - CONSQ", 1.936243593958415e-10], ["transport Alu - CONSQ", 1.5196424177717214e-10], ["avoided alubox raw materials - CONSQ", -1.1638319464952641e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.0430954980012049e-08], ["autoclave - CONSQ", 1.7848307157297192e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["market for electricity, high voltage", -1.4253562039393767e-09], ["transport Plastic - CONSQ", 5.88423518461901e-09], ["PE incineration no Energy Recovery - CONSQ", -1.5496605705058103e-11], ["PP incineration no Energy Recovery - CONSQ", -1.3628019043453102e-10], ["marginal heating grid projection updated - CONSQ", -9.508157489743055e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 1.0430954980012049e-08], ["autoclave - CONSQ", 1.7848307157297192e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.747443612396433e-10], ["market for polypropylene, granulate", -4.0611447739453945e-09], ["market for electricity, high voltage", -6.55663853812118e-10], ["transport Plastic - CONSQ", 5.88423518461901e-09], ["PE incineration no Energy Recovery - CONSQ", -7.128438624962499e-12], ["PP incineration no Energy Recovery - CONSQ", -6.26888876612392e-11], ["marginal heating grid projection updated - CONSQ", -4.3737524453639915e-09]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0005788419782701951], ["alubox production - CONSQ", 7.128328326307099e-05], ["autoclave - CONSQ", 0.0014010663180142027], ["Handwash - CONSQ", 9.14197251274628e-05], ["alubox EoL melting - CONSQ", 0.0004874946657819522], ["alubox EoL mixed sorting - CONSQ", 1.780167860430808e-05], ["transport Alu - CONSQ", 7.900768413078576e-06], ["avoided alubox raw materials - CONSQ", -0.0005375470665861999]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0008421374025219222], ["autoclave - CONSQ", 0.0014010663180142027], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["market for electricity, high voltage", -8.942695806091347e-05], ["transport Plastic - CONSQ", 0.0007600009777508464], ["PE incineration no Energy Recovery - CONSQ", -5.415379617993103e-06], ["PP incineration no Energy Recovery - CONSQ", -3.997972344788057e-05], ["marginal heating grid projection updated - CONSQ", -0.0004412712045675308]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0008421374025219222], ["autoclave - CONSQ", 0.0014010663180142027], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.223466715512621e-05], ["market for polypropylene, granulate", -0.0003344346139827557], ["market for electricity, high voltage", -4.113640070802057e-05], ["transport Plastic - CONSQ", 0.0007600009777508464], ["PE incineration no Energy Recovery - CONSQ", -2.491074624346275e-06], ["PP incineration no Energy Recovery - CONSQ", -1.8390672788989974e-05], ["marginal heating grid projection updated - CONSQ", -0.00020298475410504232]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03862284700230107], ["alubox production - CONSQ", 0.025583158377687723], ["autoclave - CONSQ", 0.04506116162085487], ["Handwash - CONSQ", 0.052961791147733764], ["alubox EoL melting - CONSQ", 0.034322357667014906], ["alubox EoL mixed sorting - CONSQ", 0.0006692049709012063], ["transport Alu - CONSQ", 0.00013773626737402736], ["avoided alubox raw materials - CONSQ", -0.03594166704133421]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.07549342364357263], ["autoclave - CONSQ", 0.04506116162085487], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["market for electricity, high voltage", -0.0028225081856488162], ["transport Plastic - CONSQ", 0.006012576485682125], ["PE incineration no Energy Recovery - CONSQ", -0.0005581463989573615], ["PP incineration no Energy Recovery - CONSQ", -0.004675623746658543], ["marginal heating grid projection updated - CONSQ", -0.016697884675900988]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.07549342364357263], ["autoclave - CONSQ", 0.04506116162085487], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.004158278213901295], ["market for polypropylene, granulate", -0.03167408291003952], ["market for electricity, high voltage", -0.001298353765398508], ["transport Plastic - CONSQ", 0.006012576485682125], ["PE incineration no Energy Recovery - CONSQ", -0.0002567473435168879], ["PP incineration no Energy Recovery - CONSQ", -0.0021507869235897125], ["marginal heating grid projection updated - CONSQ", -0.007681026951084412]]</t>
+    <t>[["alubox raw materials - CONSQ", 0.00099459313789942], ["alubox production - CONSQ", 9.762607520007814e-05], ["autoclave - CONSQ", 0.0014014285484328756], ["Handwash - CONSQ", 0.00013896506480767359], ["alubox EoL melting - CONSQ", 0.0008632211027914975], ["alubox EoL mixed sorting - CONSQ", 1.3102513601194408e-05], ["transport Alu - CONSQ", 5.11283210482023e-06], ["avoided alubox raw materials - CONSQ", -0.0009303607368585376]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955795055909], ["autoclave - CONSQ", 0.0014014285484328756], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["market for electricity, high voltage", -0.00010747647019143262], ["transport Plastic - CONSQ", 0.0005506473683008393], ["PE incineration no Energy Recovery - CONSQ", 3.975407267804606e-06], ["PP incineration no Energy Recovery - CONSQ", 2.9272704022923083e-05], ["marginal heating grid projection updated - CONSQ", -0.0003627581961719911]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0009106955795055909], ["autoclave - CONSQ", 0.0014014285484328756], ["market for corrugated board box", 3.900626665930061e-05], ["packaging film production, low density polyethylene", 9.678646032825107e-05], ["market for polypropylene, granulate", 0.0006107567782881814], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.943299789376843e-05], ["market for polypropylene, granulate", -0.00032980866027868883], ["market for electricity, high voltage", -4.9439176288059175e-05], ["transport Plastic - CONSQ", 0.0005506473683008393], ["PE incineration no Energy Recovery - CONSQ", 1.8286873430606644e-06], ["PP incineration no Energy Recovery - CONSQ", 1.3465443847277075e-05], ["marginal heating grid projection updated - CONSQ", -0.00016686877032577057]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.1542439282263658], ["alubox production - CONSQ", 0.022156774023127858], ["autoclave - CONSQ", 0.13321320200128806], ["Handwash - CONSQ", 0.02337939003610922], ["alubox EoL melting - CONSQ", 0.13106909346835469], ["alubox EoL mixed sorting - CONSQ", 0.0031809502666867344], ["transport Alu - CONSQ", 0.0021324672022102766], ["avoided alubox raw materials - CONSQ", -0.1434851961755121]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.2294040394877444], ["autoclave - CONSQ", 0.13321320200128806], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["market for electricity, high voltage", -0.005961318604063036], ["transport Plastic - CONSQ", 0.06076427765999239], ["PE incineration no Energy Recovery - CONSQ", 0.030393167090317762], ["PP incineration no Energy Recovery - CONSQ", 0.22231429048710702], ["marginal heating grid projection updated - CONSQ", -0.15272040513522483]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.2294040394877444], ["autoclave - CONSQ", 0.13321320200128806], ["market for corrugated board box", -0.001643952509815517], ["packaging film production, low density polyethylene", 0.025384539441210368], ["market for polypropylene, granulate", 0.17825063717676437], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011359305107549338], ["market for polypropylene, granulate", -0.09625534407615824], ["market for electricity, high voltage", -0.002742206557869834], ["transport Plastic - CONSQ", 0.06076427765999239], ["PE incineration no Energy Recovery - CONSQ", 0.013980856861540856], ["PP incineration no Energy Recovery - CONSQ", 0.10226457362378612], ["marginal heating grid projection updated - CONSQ", -0.0702513863654861]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.5100605935482576], ["alubox production - CONSQ", 0.11210832123122447], ["autoclave - CONSQ", 1.4495155560987139], ["Handwash - CONSQ", 1.4404517583337737], ["alubox EoL melting - CONSQ", 0.24075710947240628], ["alubox EoL mixed sorting - CONSQ", 0.017513239175713714], ["transport Alu - CONSQ", 0.01430857580692794], ["avoided alubox raw materials - CONSQ", -0.4743521447426934]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917566360178], ["autoclave - CONSQ", 1.4495155560987139], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["market for electricity, high voltage", -0.05148097890038078], ["transport Plastic - CONSQ", 0.41868503474313057], ["PE incineration no Energy Recovery - CONSQ", 0.0054926585491471515], ["PP incineration no Energy Recovery - CONSQ", 0.040469512930601914], ["marginal heating grid projection updated - CONSQ", -0.19814111317037003]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.6238917566360178], ["autoclave - CONSQ", 1.4495155560987139], ["market for corrugated board box", 0.025806817474463024], ["packaging film production, low density polyethylene", 0.03868352000395689], ["market for polypropylene, granulate", 0.21940011956150965], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.014617415777911277], ["market for polypropylene, granulate", -0.11847606457727207], ["market for electricity, high voltage", -0.023681250294174457], ["transport Plastic - CONSQ", 0.41868503474313057], ["PE incineration no Energy Recovery - CONSQ", 0.0025266229325557063], ["PP incineration no Energy Recovery - CONSQ", 0.018615975945402232], ["marginal heating grid projection updated - CONSQ", -0.09114491209864051]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.5044803926499526], ["alubox production - CONSQ", 0.33140539800866053], ["autoclave - CONSQ", 2.6222095102784126], ["Handwash - CONSQ", 0.20051845042543145], ["alubox EoL melting - CONSQ", 1.2546444967199697], ["alubox EoL mixed sorting - CONSQ", 0.03342991771883409], ["transport Alu - CONSQ", 0.03016378175177607], ["avoided alubox raw materials - CONSQ", -1.3954070272091432]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.106385068994311], ["autoclave - CONSQ", 2.6222095102784126], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["market for electricity, high voltage", -0.06451435176929034], ["transport Plastic - CONSQ", 0.76614701045209], ["PE incineration no Energy Recovery - CONSQ", 0.004737511086550725], ["PP incineration no Energy Recovery - CONSQ", 0.035315919466254855], ["marginal heating grid projection updated - CONSQ", -1.904246833360589]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 7.106385068994311], ["autoclave - CONSQ", 2.6222095102784126], ["market for corrugated board box", 0.056811625425440576], ["packaging film production, low density polyethylene", 0.8165740265774581], ["market for polypropylene, granulate", 6.398173760354218], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.3917069938836761], ["market for polypropylene, granulate", -3.455013830627775], ["market for electricity, high voltage", -0.029676601813876657], ["transport Plastic - CONSQ", 0.76614701045209], ["PE incineration no Energy Recovery - CONSQ", 0.0021792550997040234], ["PP incineration no Energy Recovery - CONSQ", 0.016245322951300968], ["marginal heating grid projection updated - CONSQ", -0.8759535433941105]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.6741804687883666e-05], ["alubox production - CONSQ", 1.3995384529203534e-05], ["autoclave - CONSQ", 3.446067564233248e-05], ["Handwash - CONSQ", 0.00018762705627212614], ["alubox EoL melting - CONSQ", 4.489880231998662e-05], ["alubox EoL mixed sorting - CONSQ", 2.9157591257047047e-06], ["transport Alu - CONSQ", 2.164169203799687e-07], ["avoided alubox raw materials - CONSQ", -5.14529755397914e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.644548399499842e-05], ["autoclave - CONSQ", 3.446067564233248e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["market for electricity, high voltage", -2.3521884456291384e-06], ["transport Plastic - CONSQ", 1.366218051763768e-05], ["PE incineration no Energy Recovery - CONSQ", 4.702523264470298e-08], ["PP incineration no Energy Recovery - CONSQ", 3.7275611969753715e-07], ["marginal heating grid projection updated - CONSQ", -2.3048939673679525e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.644548399499842e-05], ["autoclave - CONSQ", 3.446067564233248e-05], ["market for corrugated board box", 6.042636554393654e-06], ["packaging film production, low density polyethylene", 6.410903396295736e-06], ["market for polypropylene, granulate", 1.9642625111517555e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3834463252213407e-06], ["market for polypropylene, granulate", -1.0607017560192631e-05], ["market for electricity, high voltage", -1.0820066849895143e-06], ["transport Plastic - CONSQ", 1.366218051763768e-05], ["PE incineration no Energy Recovery - CONSQ", 2.163160701366802e-08], ["PP incineration no Energy Recovery - CONSQ", 1.7146781488894644e-07], ["marginal heating grid projection updated - CONSQ", -1.06025122523556e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00016388165448194658], ["alubox production - CONSQ", 2.0912907064250502e-05], ["autoclave - CONSQ", 0.0005318438006138101], ["Handwash - CONSQ", 0.00034362275809153895], ["alubox EoL melting - CONSQ", 0.0001420371138243792], ["alubox EoL mixed sorting - CONSQ", 3.0732238695277288e-06], ["transport Alu - CONSQ", 1.3826016473844613e-06], ["avoided alubox raw materials - CONSQ", -0.0001529140001265569]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256545566713], ["autoclave - CONSQ", 0.0005318438006138101], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["market for electricity, high voltage", -2.959148606151654e-05], ["transport Plastic - CONSQ", 0.00024012206522322296], ["PE incineration no Energy Recovery - CONSQ", 2.0429818248499144e-06], ["PP incineration no Energy Recovery - CONSQ", 1.4991033464436008e-05], ["marginal heating grid projection updated - CONSQ", -0.0001107407995671805]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00020091256545566713], ["autoclave - CONSQ", 0.0005318438006138101], ["market for corrugated board box", 8.382503723604798e-06], ["packaging film production, low density polyethylene", 2.1184922119661315e-05], ["market for polypropylene, granulate", 0.00012733443183989696], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.495174878614386e-06], ["market for polypropylene, granulate", -6.876059319507486e-05], ["market for electricity, high voltage", -1.3612083588297858e-05], ["transport Plastic - CONSQ", 0.00024012206522322296], ["PE incineration no Energy Recovery - CONSQ", 9.397716394177924e-07], ["PP incineration no Energy Recovery - CONSQ", 6.8958753932142505e-06], ["marginal heating grid projection updated - CONSQ", -5.094076780839811e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0017368917597659348], ["alubox production - CONSQ", 0.0001856808631600434], ["autoclave - CONSQ", 0.006227844010569461], ["Handwash - CONSQ", 0.00047487591789758035], ["alubox EoL melting - CONSQ", 0.0014965946551337395], ["alubox EoL mixed sorting - CONSQ", 3.044707377655708e-05], ["transport Alu - CONSQ", 1.4256163139493222e-05], ["avoided alubox raw materials - CONSQ", -0.0016204289389759475]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486064969478], ["autoclave - CONSQ", 0.006227844010569461], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["market for electricity, high voltage", -0.0004665919463496633], ["transport Plastic - CONSQ", 0.0026027258297973087], ["PE incineration no Energy Recovery - CONSQ", 2.085758789114653e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00015306650707853963], ["marginal heating grid projection updated - CONSQ", -0.0012188533135041506]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0021683486064969478], ["autoclave - CONSQ", 0.006227844010569461], ["market for corrugated board box", 8.462985891726445e-05], ["packaging film production, low density polyethylene", 0.00021476912661870217], ["market for polypropylene, granulate", 0.00135509540996385], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.009658202656336e-05], ["market for polypropylene, granulate", -0.0007317515213936433], ["market for electricity, high voltage", -0.00021463229532084788], ["transport Plastic - CONSQ", 0.0026027258297973087], ["PE incineration no Energy Recovery - CONSQ", 9.594490429849909e-06], ["PP incineration no Energy Recovery - CONSQ", 7.041059324972899e-05], ["marginal heating grid projection updated - CONSQ", -0.0005606725243021841]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.602823240550661e-10], ["alubox production - CONSQ", 5.309861273457702e-11], ["autoclave - CONSQ", 4.2064791570803306e-10], ["Handwash - CONSQ", 4.3228016431198623e-11], ["alubox EoL melting - CONSQ", 2.638370965891106e-10], ["alubox EoL mixed sorting - CONSQ", -1.3454077224822786e-11], ["transport Alu - CONSQ", 1.1754579074818758e-12], ["avoided alubox raw materials - CONSQ", -3.8744275372328966e-10]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115432131256e-11], ["autoclave - CONSQ", 4.2064791570803306e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["market for electricity, high voltage", -2.5871319984405878e-11], ["transport Plastic - CONSQ", 5.3489867491729446e-11], ["PE incineration no Energy Recovery - CONSQ", 7.115851260869802e-13], ["PP incineration no Energy Recovery - CONSQ", 5.494110719353825e-12], ["marginal heating grid projection updated - CONSQ", -9.417353670447324e-11]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 8.509115432131256e-11], ["autoclave - CONSQ", 4.2064791570803306e-10], ["market for corrugated board box", 5.97613015537245e-12], ["packaging film production, low density polyethylene", 1.0422277230235594e-11], ["market for polypropylene, granulate", 5.3049722076357263e-11], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.813968395074686e-12], ["market for polypropylene, granulate", -2.864684992177723e-11], ["market for electricity, high voltage", -1.190080719282235e-11], ["transport Plastic - CONSQ", 5.3489867491729446e-11], ["PE incineration no Energy Recovery - CONSQ", 3.2732915799106625e-13], ["PP incineration no Energy Recovery - CONSQ", 2.5272909296173306e-12], ["marginal heating grid projection updated - CONSQ", -4.3319826900384735e-11]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.7867630139513425e-09], ["alubox production - CONSQ", 2.906200263018611e-10], ["autoclave - CONSQ", 8.116257635880887e-09], ["Handwash - CONSQ", 1.3069705609303142e-09], ["alubox EoL melting - CONSQ", 2.0290939831383282e-09], ["alubox EoL mixed sorting - CONSQ", 1.4327769990889141e-11], ["transport Alu - CONSQ", 2.203031249356212e-11], ["avoided alubox raw materials - CONSQ", -2.6101981236571366e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.9406534290348255e-09], ["autoclave - CONSQ", 8.116257635880887e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["market for electricity, high voltage", -5.330945378301465e-10], ["transport Plastic - CONSQ", 3.9342573591988655e-10], ["PE incineration no Energy Recovery - CONSQ", 2.3717512951331163e-11], ["PP incineration no Energy Recovery - CONSQ", 1.7359564617459977e-10], ["marginal heating grid projection updated - CONSQ", -1.5653974574130285e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.9406534290348255e-09], ["autoclave - CONSQ", 8.116257635880887e-09], ["market for corrugated board box", 1.5956519890334508e-10], ["packaging film production, low density polyethylene", 1.9818498045984566e-10], ["market for polypropylene, granulate", 1.162320737396412e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.698861310212956e-11], ["market for polypropylene, granulate", -6.276531983150668e-10], ["market for electricity, high voltage", -2.452234874012752e-10], ["transport Plastic - CONSQ", 3.9342573591988655e-10], ["PE incineration no Energy Recovery - CONSQ", 1.0910055956893886e-11], ["PP incineration no Energy Recovery - CONSQ", 7.985399720897668e-11], ["marginal heating grid projection updated - CONSQ", -7.200828315440163e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0006450722461958862], ["alubox production - CONSQ", 0.0019047788568230218], ["autoclave - CONSQ", -0.005217196405826367], ["Handwash - CONSQ", 0.0017555824888882009], ["alubox EoL melting - CONSQ", 0.001246799906652905], ["alubox EoL mixed sorting - CONSQ", -0.00014755172646035883], ["transport Alu - CONSQ", 1.0961680176663579e-05], ["avoided alubox raw materials - CONSQ", -0.0006998236723237606]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999110155], ["autoclave - CONSQ", -0.005217196405826367], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["market for electricity, high voltage", -1.6945325686799705e-05], ["transport Plastic - CONSQ", 0.00027105608242653737], ["PE incineration no Energy Recovery - CONSQ", 3.1252042140617526e-07], ["PP incineration no Energy Recovery - CONSQ", 1.7490276677452454e-06], ["marginal heating grid projection updated - CONSQ", -0.009521264123083836]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008495096999110155], ["autoclave - CONSQ", -0.005217196405826367], ["market for corrugated board box", -0.0002002042908949694], ["packaging film production, low density polyethylene", 0.0013238243232220775], ["market for polypropylene, granulate", 0.0028645166075115494], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00022157206170105202], ["market for polypropylene, granulate", -0.0015468389680720798], ["market for electricity, high voltage", -7.794849815918213e-06], ["transport Plastic - CONSQ", 0.00027105608242653737], ["PE incineration no Energy Recovery - CONSQ", 1.437594042932614e-07], ["PP incineration no Energy Recovery - CONSQ", 8.045527479415564e-07], ["marginal heating grid projection updated - CONSQ", -0.004379781497145496]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.3349731984755627], ["alubox production - CONSQ", 0.3812108198418514], ["autoclave - CONSQ", 42.49728793955468], ["Handwash - CONSQ", 0.9278417162082553], ["alubox EoL melting - CONSQ", 0.17506952522890346], ["alubox EoL mixed sorting - CONSQ", 0.00402172872426269], ["transport Alu - CONSQ", 0.01874766383952674], ["avoided alubox raw materials - CONSQ", -0.2838220780851333]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591400041228], ["autoclave - CONSQ", 42.49728793955468], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["market for electricity, high voltage", -3.385238115609151], ["transport Plastic - CONSQ", 0.49202641385525475], ["PE incineration no Energy Recovery - CONSQ", -0.0005517466372827548], ["PP incineration no Energy Recovery - CONSQ", -0.003848634820686828], ["marginal heating grid projection updated - CONSQ", -4.188613611789746]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.7138591400041228], ["autoclave - CONSQ", 42.49728793955468], ["market for corrugated board box", 0.8888424244747577], ["packaging film production, low density polyethylene", 0.13536861757955918], ["market for polypropylene, granulate", 0.30578562169231066], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.01990280748454917], ["market for polypropylene, granulate", -0.16512423556264405], ["market for electricity, high voltage", -1.5572095331801954], ["transport Plastic - CONSQ", 0.49202641385525475], ["PE incineration no Energy Recovery - CONSQ", -0.0002538034539512995], ["PP incineration no Energy Recovery - CONSQ", -0.0017703720343687137], ["marginal heating grid projection updated - CONSQ", -1.9267622614630748]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.5988961825176601e-07], ["alubox production - CONSQ", 2.2129992613109264e-07], ["autoclave - CONSQ", 6.577814346858032e-06], ["Handwash - CONSQ", 1.9951477317833405e-07], ["alubox EoL melting - CONSQ", -1.0018459829525004e-06], ["alubox EoL mixed sorting - CONSQ", -2.385020641467355e-07], ["transport Alu - CONSQ", 4.20350820236115e-09], ["avoided alubox raw materials - CONSQ", -1.4329149741604288e-07]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.3437873445557385e-06], ["autoclave - CONSQ", 6.577814346858032e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["market for electricity, high voltage", -3.8494146819582574e-07], ["transport Plastic - CONSQ", -8.189405948807846e-08], ["PE incineration no Energy Recovery - CONSQ", -1.6013951476980167e-09], ["PP incineration no Energy Recovery - CONSQ", -1.3005326272564144e-08], ["marginal heating grid projection updated - CONSQ", -1.6647590283175401e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.3437873445557385e-06], ["autoclave - CONSQ", 6.577814346858032e-06], ["market for corrugated board box", 2.1164058693197575e-08], ["packaging film production, low density polyethylene", 2.1051850355073884e-07], ["market for polypropylene, granulate", 1.5874305134231447e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.0160051104600511e-07], ["market for polypropylene, granulate", -8.572124772542587e-07], ["market for electricity, high voltage", -1.7707307537004648e-07], ["transport Plastic - CONSQ", -8.189405948807846e-08], ["PE incineration no Energy Recovery - CONSQ", -7.36641770587907e-10], ["PP incineration no Energy Recovery - CONSQ", -5.982450138856097e-09], ["marginal heating grid projection updated - CONSQ", -7.65789155357081e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.3468701148877358e-09], ["alubox production - CONSQ", 6.546061518967267e-10], ["autoclave - CONSQ", 5.322695923000372e-09], ["Handwash - CONSQ", 7.056236704838176e-10], ["alubox EoL melting - CONSQ", 9.801157441678547e-10], ["alubox EoL mixed sorting - CONSQ", 8.43468971216533e-11], ["transport Alu - CONSQ", 4.8640333823231825e-11], ["avoided alubox raw materials - CONSQ", -1.2225472022151376e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.267230726978638e-09], ["autoclave - CONSQ", 5.322695923000372e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["market for electricity, high voltage", -1.2104405225218283e-10], ["transport Plastic - CONSQ", 8.958388317576703e-10], ["PE incineration no Energy Recovery - CONSQ", 1.5639344105599993e-11], ["PP incineration no Energy Recovery - CONSQ", 1.1576338348228567e-10], ["marginal heating grid projection updated - CONSQ", -1.2743144555448277e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 2.267230726978638e-09], ["autoclave - CONSQ", 5.322695923000372e-09], ["market for corrugated board box", 1.0732942519692228e-10], ["packaging film production, low density polyethylene", 5.282196376555206e-10], ["market for polypropylene, granulate", 1.4723811915819696e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.1699072692562864e-10], ["market for polypropylene, granulate", -7.950858434997455e-10], ["market for electricity, high voltage", -5.568026403590827e-11], ["transport Plastic - CONSQ", 8.958388317576703e-10], ["PE incineration no Energy Recovery - CONSQ", 7.194098288457155e-12], ["PP incineration no Energy Recovery - CONSQ", 5.3251156395736846e-11], ["marginal heating grid projection updated - CONSQ", -5.861846495544674e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.2379513986024985e-08], ["alubox production - CONSQ", 6.170387272292238e-10], ["autoclave - CONSQ", 1.7848307158013878e-08], ["Handwash - CONSQ", 2.152021349211075e-09], ["alubox EoL melting - CONSQ", 1.1187702333476039e-08], ["alubox EoL mixed sorting - CONSQ", 1.9362435940220343e-10], ["transport Alu - CONSQ", 1.5196424177591356e-10], ["avoided alubox raw materials - CONSQ", -1.1638319464784452e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.043095498051571e-08], ["autoclave - CONSQ", 1.7848307158013878e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["market for electricity, high voltage", -1.4253562039393767e-09], ["transport Plastic - CONSQ", 5.884235184588353e-09], ["PE incineration no Energy Recovery - CONSQ", 1.5496605693127887e-11], ["PP incineration no Energy Recovery - CONSQ", 1.3628019044503903e-10], ["marginal heating grid projection updated - CONSQ", -9.508157489183456e-09]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 1.043095498051571e-08], ["autoclave - CONSQ", 1.7848307158013878e-08], ["market for corrugated board box", 6.060102962883501e-10], ["packaging film production, low density polyethylene", 9.702958907333555e-10], ["market for polypropylene, granulate", 7.520638470169328e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.747443612396433e-10], ["market for polypropylene, granulate", -4.0611447739453945e-09], ["market for electricity, high voltage", -6.55663853812118e-10], ["transport Plastic - CONSQ", 5.884235184588353e-09], ["PE incineration no Energy Recovery - CONSQ", 7.128438618239559e-12], ["PP incineration no Energy Recovery - CONSQ", 6.268888757171957e-11], ["marginal heating grid projection updated - CONSQ", -4.373752445485673e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005788419782585955], ["alubox production - CONSQ", 7.128328323512274e-05], ["autoclave - CONSQ", 0.0014010663183041333], ["Handwash - CONSQ", 9.141972590600764e-05], ["alubox EoL melting - CONSQ", 0.0004874946657706408], ["alubox EoL mixed sorting - CONSQ", 1.7801678604583995e-05], ["transport Alu - CONSQ", 7.900768413038254e-06], ["avoided alubox raw materials - CONSQ", -0.0005375470665779755]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374025555673], ["autoclave - CONSQ", 0.0014010663183041333], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["market for electricity, high voltage", -8.942695806091347e-05], ["transport Plastic - CONSQ", 0.0007600009777493729], ["PE incineration no Energy Recovery - CONSQ", 5.415379617434442e-06], ["PP incineration no Energy Recovery - CONSQ", 3.9979723447892167e-05], ["marginal heating grid projection updated - CONSQ", -0.00044127120453753597]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0008421374025555673], ["autoclave - CONSQ", 0.0014010663183041333], ["market for corrugated board box", 2.859275641047564e-05], ["packaging film production, low density polyethylene", 0.0001137816437674622], ["market for polypropylene, granulate", 0.0006193233592137509], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.223466715512621e-05], ["market for polypropylene, granulate", -0.0003344346139827557], ["market for electricity, high voltage", -4.113640070802057e-05], ["transport Plastic - CONSQ", 0.0007600009777493729], ["PE incineration no Energy Recovery - CONSQ", 2.4910746239458907e-06], ["PP incineration no Energy Recovery - CONSQ", 1.839067278432401e-05], ["marginal heating grid projection updated - CONSQ", -0.00020298475411376294]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.03862284700196173], ["alubox production - CONSQ", 0.025583158376672997], ["autoclave - CONSQ", 0.04506116163029568], ["Handwash - CONSQ", 0.052961791168516445], ["alubox EoL melting - CONSQ", 0.03432235766670475], ["alubox EoL mixed sorting - CONSQ", 0.0006692049709177154], ["transport Alu - CONSQ", 0.00013773626737363821], ["avoided alubox raw materials - CONSQ", -0.03594166704109876]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.07549342364392728], ["autoclave - CONSQ", 0.04506116163029568], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["market for electricity, high voltage", -0.0028225081856488162], ["transport Plastic - CONSQ", 0.006012576485633112], ["PE incineration no Energy Recovery - CONSQ", 0.0005581463989275046], ["PP incineration no Energy Recovery - CONSQ", 0.004675623746638889], ["marginal heating grid projection updated - CONSQ", -0.016697884675243062]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.07549342364392728], ["autoclave - CONSQ", 0.04506116163029568], ["market for corrugated board box", 0.0019124220055341606], ["packaging film production, low density polyethylene", 0.019129675350616448], ["market for polypropylene, granulate", 0.05865570909259933], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.004158278213901295], ["market for polypropylene, granulate", -0.03167408291003952], ["market for electricity, high voltage", -0.001298353765398508], ["transport Plastic - CONSQ", 0.006012576485633112], ["PE incineration no Energy Recovery - CONSQ", 0.00025674734350539696], ["PP incineration no Energy Recovery - CONSQ", 0.002150786923382669], ["marginal heating grid projection updated - CONSQ", -0.007681026951166853]]</t>
   </si>
 </sst>
 </file>

</xml_diff>